<commit_message>
Finsihing with the second video, up to some corrections coming up.
</commit_message>
<xml_diff>
--- a/PresentValueSeries/CF_CH_2021_12.xlsx
+++ b/PresentValueSeries/CF_CH_2021_12.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="494" documentId="115_{3C012DFA-6514-47FB-A009-009EE274F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CB0E92D-EE33-4C7E-8DD9-A103383EBB92}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39869210-F43E-4495-BAE7-54453A6509FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4250" yWindow="1430" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="13460" windowHeight="6570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>ReportingNode</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>GIC1_CH</t>
+  </si>
+  <si>
+    <t>AccidentYear</t>
   </si>
 </sst>
 </file>
@@ -1114,13 +1117,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BM9" totalsRowShown="0">
-  <autoFilter ref="A1:BM9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BN9" totalsRowShown="0">
+  <autoFilter ref="A1:BN9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="66">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DataNode" dataDxfId="64"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="AmountType" dataDxfId="63"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="AocType" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Novelty" dataDxfId="61"/>
+    <tableColumn id="66" xr3:uid="{683B5F91-AC14-480B-B60D-EBABB784381F}" name="AccidentYear"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Values0" dataDxfId="60"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Values1" dataDxfId="59"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Values2" dataDxfId="58"/>
@@ -1486,7 +1490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF902ED-C214-4F96-9503-445B7BE7E04C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1537,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59E8FC3-4B20-424B-A44D-77DCF1F6F0A1}">
-  <dimension ref="A1:BU17"/>
+  <dimension ref="A1:BV17"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1549,11 +1553,12 @@
     <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="65" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="6" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="66" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1567,190 +1572,193 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>51</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>53</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>54</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>56</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>57</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>58</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>59</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>60</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>61</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>62</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>63</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>64</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>65</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>66</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>67</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>68</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>69</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>70</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>71</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>72</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>73</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>74</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>75</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>76</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>77</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>78</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>79</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -1763,190 +1771,189 @@
       <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>80</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>80.079999999999984</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>80.240159999999989</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>80.480880479999982</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>80.802804001919981</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>81.206818021929578</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>81.694058930061161</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>82.265917342571584</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>82.924044681312154</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>83.67036108344395</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="3">
         <v>84.507064694278384</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>85.521149470609728</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="3">
         <v>86.718445563198259</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="3">
         <v>88.10594069220943</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="3">
         <v>89.691847624669194</v>
       </c>
-      <c r="T2" s="3">
+      <c r="U2" s="3">
         <v>91.485684577162573</v>
       </c>
-      <c r="U2" s="3">
+      <c r="V2" s="3">
         <v>93.498369637860151</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="3">
         <v>95.742330509168795</v>
       </c>
-      <c r="W2" s="3">
+      <c r="X2" s="3">
         <v>98.423115763425528</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Y2" s="3">
         <v>101.57265546785514</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Z2" s="3">
         <v>105.22927106469793</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="3">
         <v>109.43844190728585</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AB2" s="3">
         <v>114.25373335120644</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AC2" s="3">
         <v>119.73791255206434</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AD2" s="3">
         <v>125.9642840047717</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AE2" s="3">
         <v>133.01828390903893</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AF2" s="3">
         <v>141.13239922749028</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AG2" s="3">
         <v>150.44713757650464</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AH2" s="3">
         <v>161.12888434443647</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AI2" s="3">
         <v>173.37467955461366</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AJ2" s="3">
         <v>187.41802859853738</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AK2" s="3">
         <v>203.53597905801161</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AL2" s="3">
         <v>222.05775315229064</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AM2" s="3">
         <v>243.37529745491057</v>
       </c>
-      <c r="AM2" s="3">
+      <c r="AN2" s="3">
         <v>266.2525754156722</v>
       </c>
-      <c r="AN2" s="3">
+      <c r="AO2" s="3">
         <v>290.48155977849837</v>
       </c>
-      <c r="AO2" s="3">
+      <c r="AP2" s="3">
         <v>315.75345547922774</v>
       </c>
-      <c r="AP2" s="3">
+      <c r="AQ2" s="3">
         <v>341.96099228400362</v>
       </c>
-      <c r="AQ2" s="3">
+      <c r="AR2" s="3">
         <v>368.97591067443989</v>
       </c>
-      <c r="AR2" s="3">
+      <c r="AS2" s="3">
         <v>396.28012806434845</v>
       </c>
-      <c r="AS2" s="3">
+      <c r="AT2" s="3">
         <v>423.62345690078848</v>
       </c>
-      <c r="AT2" s="3">
+      <c r="AU2" s="3">
         <v>450.735358142439</v>
       </c>
-      <c r="AU2" s="3">
+      <c r="AV2" s="3">
         <v>476.8780089147005</v>
       </c>
-      <c r="AV2" s="3">
+      <c r="AW2" s="3">
         <v>501.67566537826497</v>
       </c>
-      <c r="AW2" s="3">
+      <c r="AX2" s="3">
         <v>523.74939465490866</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="AY2" s="3">
         <v>542.08062346783038</v>
       </c>
-      <c r="AY2" s="3">
+      <c r="AZ2" s="3">
         <v>555.0905584310583</v>
       </c>
-      <c r="AZ2" s="3">
+      <c r="BA2" s="3">
         <v>561.75164513223103</v>
       </c>
-      <c r="BA2" s="3">
+      <c r="BB2" s="3">
         <v>563.43690006762768</v>
       </c>
-      <c r="BB2" s="3">
+      <c r="BC2" s="3">
         <v>560.05627866722193</v>
       </c>
-      <c r="BC2" s="3">
+      <c r="BD2" s="3">
         <v>546.61492797920857</v>
       </c>
-      <c r="BD2" s="3">
+      <c r="BE2" s="3">
         <v>510.53834273258076</v>
       </c>
-      <c r="BE2" s="3">
+      <c r="BF2" s="3">
         <v>463.56881520118333</v>
       </c>
-      <c r="BF2" s="3">
+      <c r="BG2" s="3">
         <v>407.01341974663899</v>
       </c>
-      <c r="BG2" s="3">
+      <c r="BH2" s="3">
         <v>343.11231284641667</v>
       </c>
-      <c r="BH2" s="3">
+      <c r="BI2" s="3">
         <v>275.51918721567256</v>
       </c>
-      <c r="BI2" s="3">
+      <c r="BJ2" s="3">
         <v>207.46594797340143</v>
       </c>
-      <c r="BJ2" s="3">
+      <c r="BK2" s="3">
         <v>143.77390194556719</v>
       </c>
-      <c r="BK2" s="3">
+      <c r="BL2" s="3">
         <v>89.571140912088353</v>
       </c>
-      <c r="BL2" s="3">
+      <c r="BM2" s="3">
         <v>46.576993274285947</v>
       </c>
-      <c r="BM2" s="3">
+      <c r="BN2" s="3">
         <v>13.973097982285781</v>
       </c>
-      <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1"/>
@@ -1954,8 +1961,9 @@
       <c r="BS2" s="1"/>
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
-    </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV2" s="1"/>
+    </row>
+    <row r="3" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1968,190 +1976,189 @@
       <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>73.600000000000009</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>73.804183056030055</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>74.005988873511555</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>74.269718768748874</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>74.602103085421973</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>75.006373842903812</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>75.484843073551531</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>76.039564981379542</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>76.672583056089877</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>77.386045313005297</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>78.182267965644314</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>79.162546254399487</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>80.310070532763987</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>81.632147903865302</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>83.137014389372965</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>84.833991199275289</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>86.733618778901089</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>88.847787214432557</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>91.398523020198041</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>94.38378902608703</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>97.84048680705294</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>101.81202532505596</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>106.34926686943705</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>111.51162183060511</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>117.36833499037918</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>124.00000655936267</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>131.63924730391071</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="3">
         <v>140.40441871180292</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AH3" s="3">
         <v>150.45251100323148</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AI3" s="3">
         <v>161.96935505694907</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AJ3" s="3">
         <v>175.17511790862838</v>
       </c>
-      <c r="AJ3" s="3">
+      <c r="AK3" s="3">
         <v>190.33099133776699</v>
       </c>
-      <c r="AK3" s="3">
+      <c r="AL3" s="3">
         <v>207.74734818051408</v>
       </c>
-      <c r="AL3" s="3">
+      <c r="AM3" s="3">
         <v>227.79370894463409</v>
       </c>
-      <c r="AM3" s="3">
+      <c r="AN3" s="3">
         <v>249.16177239767649</v>
       </c>
-      <c r="AN3" s="3">
+      <c r="AO3" s="3">
         <v>271.76161553762893</v>
       </c>
-      <c r="AO3" s="3">
+      <c r="AP3" s="3">
         <v>295.29571363611007</v>
       </c>
-      <c r="AP3" s="3">
+      <c r="AQ3" s="3">
         <v>319.68428445689688</v>
       </c>
-      <c r="AQ3" s="3">
+      <c r="AR3" s="3">
         <v>344.80562754757858</v>
       </c>
-      <c r="AR3" s="3">
+      <c r="AS3" s="3">
         <v>370.13651614737176</v>
       </c>
-      <c r="AS3" s="3">
+      <c r="AT3" s="3">
         <v>395.47166973057449</v>
       </c>
-      <c r="AT3" s="3">
+      <c r="AU3" s="3">
         <v>420.55648958365617</v>
       </c>
-      <c r="AU3" s="3">
+      <c r="AV3" s="3">
         <v>444.64998164767547</v>
       </c>
-      <c r="AV3" s="3">
+      <c r="AW3" s="3">
         <v>467.44073541042076</v>
       </c>
-      <c r="AW3" s="3">
+      <c r="AX3" s="3">
         <v>487.51460902938481</v>
       </c>
-      <c r="AX3" s="3">
+      <c r="AY3" s="3">
         <v>503.94367963936435</v>
       </c>
-      <c r="AY3" s="3">
+      <c r="AZ3" s="3">
         <v>515.11768679476836</v>
       </c>
-      <c r="AZ3" s="3">
+      <c r="BA3" s="3">
         <v>519.98471567021829</v>
       </c>
-      <c r="BA3" s="3">
+      <c r="BB3" s="3">
         <v>519.95330893972323</v>
       </c>
-      <c r="BB3" s="3">
+      <c r="BC3" s="3">
         <v>517.48879736462914</v>
       </c>
-      <c r="BC3" s="3">
+      <c r="BD3" s="3">
         <v>507.25239871488412</v>
       </c>
-      <c r="BD3" s="3">
+      <c r="BE3" s="3">
         <v>476.45864451893556</v>
       </c>
-      <c r="BE3" s="3">
+      <c r="BF3" s="3">
         <v>433.73385895599188</v>
       </c>
-      <c r="BF3" s="3">
+      <c r="BG3" s="3">
         <v>381.78314678385362</v>
       </c>
-      <c r="BG3" s="3">
+      <c r="BH3" s="3">
         <v>322.67382619765033</v>
       </c>
-      <c r="BH3" s="3">
+      <c r="BI3" s="3">
         <v>259.78356161859261</v>
       </c>
-      <c r="BI3" s="3">
+      <c r="BJ3" s="3">
         <v>196.18556690700947</v>
       </c>
-      <c r="BJ3" s="3">
+      <c r="BK3" s="3">
         <v>136.3798155198939</v>
       </c>
-      <c r="BK3" s="3">
+      <c r="BL3" s="3">
         <v>85.241419067552911</v>
       </c>
-      <c r="BL3" s="3">
+      <c r="BM3" s="3">
         <v>44.514839598436339</v>
       </c>
-      <c r="BM3" s="3">
+      <c r="BN3" s="3">
         <v>13.458093512555834</v>
       </c>
-      <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
@@ -2159,8 +2166,9 @@
       <c r="BS3" s="1"/>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
-    </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV3" s="1"/>
+    </row>
+    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
@@ -2173,190 +2181,189 @@
       <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>80</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>80.221938104380499</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>80.441292253816911</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>80.727955183422679</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>81.089242484154312</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>81.528667220547618</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>82.048742471251657</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>82.651701066716882</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>83.33976419140204</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>84.115266644570966</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>84.980726049613381</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>86.046245928695086</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>87.293554926917366</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>88.73059554767967</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="3">
         <v>90.366319988448865</v>
       </c>
-      <c r="T4" s="3">
+      <c r="U4" s="3">
         <v>92.210859999212261</v>
       </c>
-      <c r="U4" s="3">
+      <c r="V4" s="3">
         <v>94.275672585762052</v>
       </c>
-      <c r="V4" s="3">
+      <c r="W4" s="3">
         <v>96.573681754817997</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="3">
         <v>99.346220674128304</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Y4" s="3">
         <v>102.59107502835546</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Z4" s="3">
         <v>106.34835522505755</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AA4" s="3">
         <v>110.66524491853907</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="3">
         <v>115.59702920590982</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AC4" s="3">
         <v>121.2082845984838</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AD4" s="3">
         <v>127.57427716345563</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AE4" s="3">
         <v>134.7826158253942</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AF4" s="3">
         <v>143.08613837381597</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AG4" s="3">
         <v>152.61349859978577</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AH4" s="3">
         <v>163.53533804699072</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AI4" s="3">
         <v>176.05364680103159</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AJ4" s="3">
         <v>190.40773685720475</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AK4" s="3">
         <v>206.88151232365976</v>
       </c>
-      <c r="AK4" s="3">
+      <c r="AL4" s="3">
         <v>225.81233497881965</v>
       </c>
-      <c r="AL4" s="3">
+      <c r="AM4" s="3">
         <v>247.60185754851531</v>
       </c>
-      <c r="AM4" s="3">
+      <c r="AN4" s="3">
         <v>270.8280134757353</v>
       </c>
-      <c r="AN4" s="3">
+      <c r="AO4" s="3">
         <v>295.39306036698792</v>
       </c>
-      <c r="AO4" s="3">
+      <c r="AP4" s="3">
         <v>320.9736017783805</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AQ4" s="3">
         <v>347.48291788793136</v>
       </c>
-      <c r="AQ4" s="3">
+      <c r="AR4" s="3">
         <v>374.78872559519408</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AS4" s="3">
         <v>402.32230016018667</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AT4" s="3">
         <v>429.86051057671136</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AU4" s="3">
         <v>457.12661911266974</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AV4" s="3">
         <v>483.3151974431255</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AW4" s="3">
         <v>508.08775588089208</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AX4" s="3">
         <v>529.90718372759216</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AY4" s="3">
         <v>547.76486917322211</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AZ4" s="3">
         <v>559.91052912474822</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="BA4" s="3">
         <v>565.20077790241112</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BB4" s="3">
         <v>565.16664015187303</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BC4" s="3">
         <v>562.487823222423</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BD4" s="3">
         <v>551.36130295096098</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BE4" s="3">
         <v>517.88983099884297</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BF4" s="3">
         <v>471.44984669129548</v>
       </c>
-      <c r="BF4" s="3">
+      <c r="BG4" s="3">
         <v>414.98168128679742</v>
       </c>
-      <c r="BG4" s="3">
+      <c r="BH4" s="3">
         <v>350.73241978005467</v>
       </c>
-      <c r="BH4" s="3">
+      <c r="BI4" s="3">
         <v>282.37343654194848</v>
       </c>
-      <c r="BI4" s="3">
+      <c r="BJ4" s="3">
         <v>213.24518142066248</v>
       </c>
-      <c r="BJ4" s="3">
+      <c r="BK4" s="3">
         <v>148.23892991292814</v>
       </c>
-      <c r="BK4" s="3">
+      <c r="BL4" s="3">
         <v>92.653716377774899</v>
       </c>
-      <c r="BL4" s="3">
+      <c r="BM4" s="3">
         <v>48.385695215691669</v>
       </c>
-      <c r="BM4" s="3">
+      <c r="BN4" s="3">
         <v>14.628362513647645</v>
       </c>
-      <c r="BN4" s="1"/>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
@@ -2364,8 +2371,9 @@
       <c r="BS4" s="1"/>
       <c r="BT4" s="1"/>
       <c r="BU4" s="1"/>
-    </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV4" s="1"/>
+    </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
@@ -2378,190 +2386,189 @@
       <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>80</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>80.221938104380499</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>80.441292253816911</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>80.727955183422679</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>81.089242484154312</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>81.528667220547618</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>82.048742471251657</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>82.651701066716882</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>83.33976419140204</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>84.115266644570966</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>84.980726049613381</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="3">
         <v>86.046245928695086</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>87.293554926917366</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="3">
         <v>88.73059554767967</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="3">
         <v>90.366319988448865</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="3">
         <v>92.210859999212261</v>
       </c>
-      <c r="U5" s="3">
+      <c r="V5" s="3">
         <v>94.275672585762052</v>
       </c>
-      <c r="V5" s="3">
+      <c r="W5" s="3">
         <v>96.573681754817997</v>
       </c>
-      <c r="W5" s="3">
+      <c r="X5" s="3">
         <v>99.346220674128304</v>
       </c>
-      <c r="X5" s="3">
+      <c r="Y5" s="3">
         <v>102.59107502835546</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Z5" s="3">
         <v>106.34835522505755</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="AA5" s="3">
         <v>110.66524491853907</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AB5" s="3">
         <v>115.59702920590982</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AC5" s="3">
         <v>121.2082845984838</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="AD5" s="3">
         <v>127.57427716345563</v>
       </c>
-      <c r="AD5" s="3">
+      <c r="AE5" s="3">
         <v>134.7826158253942</v>
       </c>
-      <c r="AE5" s="3">
+      <c r="AF5" s="3">
         <v>143.08613837381597</v>
       </c>
-      <c r="AF5" s="3">
+      <c r="AG5" s="3">
         <v>152.61349859978577</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AH5" s="3">
         <v>163.53533804699072</v>
       </c>
-      <c r="AH5" s="3">
+      <c r="AI5" s="3">
         <v>176.05364680103159</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AJ5" s="3">
         <v>190.40773685720475</v>
       </c>
-      <c r="AJ5" s="3">
+      <c r="AK5" s="3">
         <v>206.88151232365976</v>
       </c>
-      <c r="AK5" s="3">
+      <c r="AL5" s="3">
         <v>225.81233497881965</v>
       </c>
-      <c r="AL5" s="3">
+      <c r="AM5" s="3">
         <v>247.60185754851531</v>
       </c>
-      <c r="AM5" s="3">
+      <c r="AN5" s="3">
         <v>270.8280134757353</v>
       </c>
-      <c r="AN5" s="3">
+      <c r="AO5" s="3">
         <v>295.39306036698792</v>
       </c>
-      <c r="AO5" s="3">
+      <c r="AP5" s="3">
         <v>320.9736017783805</v>
       </c>
-      <c r="AP5" s="3">
+      <c r="AQ5" s="3">
         <v>347.48291788793136</v>
       </c>
-      <c r="AQ5" s="3">
+      <c r="AR5" s="3">
         <v>374.78872559519408</v>
       </c>
-      <c r="AR5" s="3">
+      <c r="AS5" s="3">
         <v>402.32230016018667</v>
       </c>
-      <c r="AS5" s="3">
+      <c r="AT5" s="3">
         <v>429.86051057671136</v>
       </c>
-      <c r="AT5" s="3">
+      <c r="AU5" s="3">
         <v>457.12661911266974</v>
       </c>
-      <c r="AU5" s="3">
+      <c r="AV5" s="3">
         <v>483.3151974431255</v>
       </c>
-      <c r="AV5" s="3">
+      <c r="AW5" s="3">
         <v>508.08775588089208</v>
       </c>
-      <c r="AW5" s="3">
+      <c r="AX5" s="3">
         <v>529.90718372759216</v>
       </c>
-      <c r="AX5" s="3">
+      <c r="AY5" s="3">
         <v>547.76486917322211</v>
       </c>
-      <c r="AY5" s="3">
+      <c r="AZ5" s="3">
         <v>559.91052912474822</v>
       </c>
-      <c r="AZ5" s="3">
+      <c r="BA5" s="3">
         <v>565.20077790241112</v>
       </c>
-      <c r="BA5" s="3">
+      <c r="BB5" s="3">
         <v>565.16664015187303</v>
       </c>
-      <c r="BB5" s="3">
+      <c r="BC5" s="3">
         <v>562.487823222423</v>
       </c>
-      <c r="BC5" s="3">
+      <c r="BD5" s="3">
         <v>551.36130295096098</v>
       </c>
-      <c r="BD5" s="3">
+      <c r="BE5" s="3">
         <v>517.88983099884297</v>
       </c>
-      <c r="BE5" s="3">
+      <c r="BF5" s="3">
         <v>471.44984669129548</v>
       </c>
-      <c r="BF5" s="3">
+      <c r="BG5" s="3">
         <v>414.98168128679742</v>
       </c>
-      <c r="BG5" s="3">
+      <c r="BH5" s="3">
         <v>350.73241978005467</v>
       </c>
-      <c r="BH5" s="3">
+      <c r="BI5" s="3">
         <v>282.37343654194848</v>
       </c>
-      <c r="BI5" s="3">
+      <c r="BJ5" s="3">
         <v>213.24518142066248</v>
       </c>
-      <c r="BJ5" s="3">
+      <c r="BK5" s="3">
         <v>148.23892991292814</v>
       </c>
-      <c r="BK5" s="3">
+      <c r="BL5" s="3">
         <v>92.653716377774899</v>
       </c>
-      <c r="BL5" s="3">
+      <c r="BM5" s="3">
         <v>48.385695215691669</v>
       </c>
-      <c r="BM5" s="3">
+      <c r="BN5" s="3">
         <v>14.628362513647645</v>
       </c>
-      <c r="BN5" s="1"/>
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
@@ -2569,8 +2576,9 @@
       <c r="BS5" s="1"/>
       <c r="BT5" s="1"/>
       <c r="BU5" s="1"/>
-    </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV5" s="1"/>
+    </row>
+    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
@@ -2583,190 +2591,189 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>-2210.5500000000002</v>
       </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
       <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
         <v>-1989.4950000000001</v>
       </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
       <c r="J6" s="3">
         <v>0</v>
       </c>
       <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
         <v>-1790.5455000000002</v>
       </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
       <c r="M6" s="3">
         <v>0</v>
       </c>
       <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
         <v>-1611.4909500000001</v>
       </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
       <c r="P6" s="3">
         <v>0</v>
       </c>
       <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
         <v>-1450.3418550000001</v>
       </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
       <c r="S6" s="3">
         <v>0</v>
       </c>
       <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
         <v>-1305.3076695000002</v>
       </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
       <c r="V6" s="3">
         <v>0</v>
       </c>
       <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
         <v>-1174.7769025500002</v>
       </c>
-      <c r="X6" s="3">
-        <v>0</v>
-      </c>
       <c r="Y6" s="3">
         <v>0</v>
       </c>
       <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
         <v>-1057.2992122950002</v>
       </c>
-      <c r="AA6" s="3">
-        <v>0</v>
-      </c>
       <c r="AB6" s="3">
         <v>0</v>
       </c>
       <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
         <v>-951.56929106550024</v>
       </c>
-      <c r="AD6" s="3">
-        <v>0</v>
-      </c>
       <c r="AE6" s="3">
         <v>0</v>
       </c>
       <c r="AF6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
         <v>-856.41236195895021</v>
       </c>
-      <c r="AG6" s="3">
-        <v>0</v>
-      </c>
       <c r="AH6" s="3">
         <v>0</v>
       </c>
       <c r="AI6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="3">
         <v>-770.77112576305524</v>
       </c>
-      <c r="AJ6" s="3">
-        <v>0</v>
-      </c>
       <c r="AK6" s="3">
         <v>0</v>
       </c>
       <c r="AL6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="3">
         <v>-693.69401318674977</v>
       </c>
-      <c r="AM6" s="3">
-        <v>0</v>
-      </c>
       <c r="AN6" s="3">
         <v>0</v>
       </c>
       <c r="AO6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="3">
         <v>-624.32461186807484</v>
       </c>
-      <c r="AP6" s="3">
-        <v>0</v>
-      </c>
       <c r="AQ6" s="3">
         <v>0</v>
       </c>
       <c r="AR6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="3">
         <v>-555.64890456258661</v>
       </c>
-      <c r="AS6" s="3">
-        <v>0</v>
-      </c>
       <c r="AT6" s="3">
         <v>0</v>
       </c>
       <c r="AU6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="3">
         <v>-483.41454696945033</v>
       </c>
-      <c r="AV6" s="3">
-        <v>0</v>
-      </c>
       <c r="AW6" s="3">
         <v>0</v>
       </c>
       <c r="AX6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="3">
         <v>-406.06821945433825</v>
       </c>
-      <c r="AY6" s="3">
-        <v>0</v>
-      </c>
       <c r="AZ6" s="3">
         <v>0</v>
       </c>
       <c r="BA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="3">
         <v>-324.85457556347063</v>
       </c>
-      <c r="BB6" s="3">
-        <v>0</v>
-      </c>
       <c r="BC6" s="3">
         <v>0</v>
       </c>
       <c r="BD6" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="3">
         <v>-243.64093167260296</v>
       </c>
-      <c r="BE6" s="3">
-        <v>0</v>
-      </c>
       <c r="BF6" s="3">
         <v>0</v>
       </c>
       <c r="BG6" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="3">
         <v>-168.11224285409602</v>
       </c>
-      <c r="BH6" s="3">
-        <v>0</v>
-      </c>
       <c r="BI6" s="3">
         <v>0</v>
       </c>
       <c r="BJ6" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="3">
         <v>-104.22959056953954</v>
       </c>
-      <c r="BK6" s="3">
-        <v>0</v>
-      </c>
       <c r="BL6" s="3">
         <v>0</v>
       </c>
       <c r="BM6" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="3">
         <v>-56.283978907551358</v>
       </c>
-      <c r="BN6" s="1"/>
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
@@ -2774,8 +2781,9 @@
       <c r="BS6" s="1"/>
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
-    </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV6" s="1"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>82</v>
       </c>
@@ -2788,190 +2796,189 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>-2210.5500000000002</v>
       </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
       <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
         <v>-2063.2215160144488</v>
       </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
       <c r="J7" s="3">
         <v>0</v>
       </c>
       <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
         <v>-1882.8080036188367</v>
       </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
       <c r="M7" s="3">
         <v>0</v>
       </c>
       <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
         <v>-1709.2914496442083</v>
       </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
       <c r="P7" s="3">
         <v>0</v>
       </c>
       <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
         <v>-1548.107757870913</v>
       </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
       <c r="S7" s="3">
         <v>0</v>
       </c>
       <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
         <v>-1400.2266747581864</v>
       </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
       <c r="V7" s="3">
         <v>0</v>
       </c>
       <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
         <v>-1265.3600787277182</v>
       </c>
-      <c r="X7" s="3">
-        <v>0</v>
-      </c>
       <c r="Y7" s="3">
         <v>0</v>
       </c>
       <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
         <v>-1142.6680434267498</v>
       </c>
-      <c r="AA7" s="3">
-        <v>0</v>
-      </c>
       <c r="AB7" s="3">
         <v>0</v>
       </c>
       <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
         <v>-1031.1590303291489</v>
       </c>
-      <c r="AD7" s="3">
-        <v>0</v>
-      </c>
       <c r="AE7" s="3">
         <v>0</v>
       </c>
       <c r="AF7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
         <v>-930.12425790876898</v>
       </c>
-      <c r="AG7" s="3">
-        <v>0</v>
-      </c>
       <c r="AH7" s="3">
         <v>0</v>
       </c>
       <c r="AI7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="3">
         <v>-838.69960468102829</v>
       </c>
-      <c r="AJ7" s="3">
-        <v>0</v>
-      </c>
       <c r="AK7" s="3">
         <v>0</v>
       </c>
       <c r="AL7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="3">
         <v>-755.89487156573273</v>
       </c>
-      <c r="AM7" s="3">
-        <v>0</v>
-      </c>
       <c r="AN7" s="3">
         <v>0</v>
       </c>
       <c r="AO7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="3">
         <v>-681.03269727904706</v>
       </c>
-      <c r="AP7" s="3">
-        <v>0</v>
-      </c>
       <c r="AQ7" s="3">
         <v>0</v>
       </c>
       <c r="AR7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="3">
         <v>-606.47057787820472</v>
       </c>
-      <c r="AS7" s="3">
-        <v>0</v>
-      </c>
       <c r="AT7" s="3">
         <v>0</v>
       </c>
       <c r="AU7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="3">
         <v>-527.46046281648682</v>
       </c>
-      <c r="AV7" s="3">
-        <v>0</v>
-      </c>
       <c r="AW7" s="3">
         <v>0</v>
       </c>
       <c r="AX7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="3">
         <v>-441.49550282763306</v>
       </c>
-      <c r="AY7" s="3">
-        <v>0</v>
-      </c>
       <c r="AZ7" s="3">
         <v>0</v>
       </c>
       <c r="BA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="3">
         <v>-342.98899321869982</v>
       </c>
-      <c r="BB7" s="3">
-        <v>0</v>
-      </c>
       <c r="BC7" s="3">
         <v>0</v>
       </c>
       <c r="BD7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="3">
         <v>-269.66796579728577</v>
       </c>
-      <c r="BE7" s="3">
-        <v>0</v>
-      </c>
       <c r="BF7" s="3">
         <v>0</v>
       </c>
       <c r="BG7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="3">
         <v>-189.73508154216125</v>
       </c>
-      <c r="BH7" s="3">
-        <v>0</v>
-      </c>
       <c r="BI7" s="3">
         <v>0</v>
       </c>
       <c r="BJ7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="3">
         <v>-119.40335697364351</v>
       </c>
-      <c r="BK7" s="3">
-        <v>0</v>
-      </c>
       <c r="BL7" s="3">
         <v>0</v>
       </c>
       <c r="BM7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="3">
         <v>-65.653826382205708</v>
       </c>
-      <c r="BN7" s="1"/>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
@@ -2979,8 +2986,9 @@
       <c r="BS7" s="1"/>
       <c r="BT7" s="1"/>
       <c r="BU7" s="1"/>
-    </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV7" s="1"/>
+    </row>
+    <row r="8" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>82</v>
       </c>
@@ -2993,190 +3001,189 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>-2210.5500000000002</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
       <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
         <v>-1936.0518028052484</v>
       </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
       <c r="J8" s="3">
         <v>0</v>
       </c>
       <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
         <v>-1721.4454032739382</v>
       </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
       <c r="M8" s="3">
         <v>0</v>
       </c>
       <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
         <v>-1536.7528388427074</v>
       </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
       <c r="P8" s="3">
         <v>0</v>
       </c>
       <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
         <v>-1374.5375449647067</v>
       </c>
-      <c r="R8" s="3">
-        <v>0</v>
-      </c>
       <c r="S8" s="3">
         <v>0</v>
       </c>
       <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
         <v>-1230.8726159976718</v>
       </c>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
       <c r="V8" s="3">
         <v>0</v>
       </c>
       <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
         <v>-1103.0807329563593</v>
       </c>
-      <c r="X8" s="3">
-        <v>0</v>
-      </c>
       <c r="Y8" s="3">
         <v>0</v>
       </c>
       <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
         <v>-989.21394837205116</v>
       </c>
-      <c r="AA8" s="3">
-        <v>0</v>
-      </c>
       <c r="AB8" s="3">
         <v>0</v>
       </c>
       <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
         <v>-887.70944819490865</v>
       </c>
-      <c r="AD8" s="3">
-        <v>0</v>
-      </c>
       <c r="AE8" s="3">
         <v>0</v>
       </c>
       <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
         <v>-796.97075391664043</v>
       </c>
-      <c r="AG8" s="3">
-        <v>0</v>
-      </c>
       <c r="AH8" s="3">
         <v>0</v>
       </c>
       <c r="AI8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="3">
         <v>-715.76055114107919</v>
       </c>
-      <c r="AJ8" s="3">
-        <v>0</v>
-      </c>
       <c r="AK8" s="3">
         <v>0</v>
       </c>
       <c r="AL8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="3">
         <v>-643.16297729171379</v>
       </c>
-      <c r="AM8" s="3">
-        <v>0</v>
-      </c>
       <c r="AN8" s="3">
         <v>0</v>
       </c>
       <c r="AO8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="3">
         <v>-578.14594308184928</v>
       </c>
-      <c r="AP8" s="3">
-        <v>0</v>
-      </c>
       <c r="AQ8" s="3">
         <v>0</v>
       </c>
       <c r="AR8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="3">
         <v>-514.21020439099971</v>
       </c>
-      <c r="AS8" s="3">
-        <v>0</v>
-      </c>
       <c r="AT8" s="3">
         <v>0</v>
       </c>
       <c r="AU8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="3">
         <v>-447.52622922857421</v>
       </c>
-      <c r="AV8" s="3">
-        <v>0</v>
-      </c>
       <c r="AW8" s="3">
         <v>0</v>
       </c>
       <c r="AX8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="3">
         <v>-377.43031433438631</v>
       </c>
-      <c r="AY8" s="3">
-        <v>0</v>
-      </c>
       <c r="AZ8" s="3">
         <v>0</v>
       </c>
       <c r="BA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="3">
         <v>-311.14322108830936</v>
       </c>
-      <c r="BB8" s="3">
-        <v>0</v>
-      </c>
       <c r="BC8" s="3">
         <v>0</v>
       </c>
       <c r="BD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="3">
         <v>-221.75414952256722</v>
       </c>
-      <c r="BE8" s="3">
-        <v>0</v>
-      </c>
       <c r="BF8" s="3">
         <v>0</v>
       </c>
       <c r="BG8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="3">
         <v>-149.14518180503313</v>
       </c>
-      <c r="BH8" s="3">
-        <v>0</v>
-      </c>
       <c r="BI8" s="3">
         <v>0</v>
       </c>
       <c r="BJ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="3">
         <v>-90.491507554494788</v>
       </c>
-      <c r="BK8" s="3">
-        <v>0</v>
-      </c>
       <c r="BL8" s="3">
         <v>0</v>
       </c>
       <c r="BM8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="3">
         <v>-47.475045860823556</v>
       </c>
-      <c r="BN8" s="1"/>
       <c r="BO8" s="1"/>
       <c r="BP8" s="1"/>
       <c r="BQ8" s="1"/>
@@ -3184,8 +3191,9 @@
       <c r="BS8" s="1"/>
       <c r="BT8" s="1"/>
       <c r="BU8" s="1"/>
-    </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="BV8" s="1"/>
+    </row>
+    <row r="9" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -3198,190 +3206,189 @@
       <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>-2210.5500000000002</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
       <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
         <v>-1936.0518028052484</v>
       </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
       <c r="J9" s="3">
         <v>0</v>
       </c>
       <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
         <v>-1721.4454032739382</v>
       </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
       <c r="M9" s="3">
         <v>0</v>
       </c>
       <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
         <v>-1536.7528388427074</v>
       </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
       <c r="P9" s="3">
         <v>0</v>
       </c>
       <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
         <v>-1374.5375449647067</v>
       </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
       <c r="S9" s="3">
         <v>0</v>
       </c>
       <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
         <v>-1230.8726159976718</v>
       </c>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
       <c r="V9" s="3">
         <v>0</v>
       </c>
       <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
         <v>-1103.0807329563593</v>
       </c>
-      <c r="X9" s="3">
-        <v>0</v>
-      </c>
       <c r="Y9" s="3">
         <v>0</v>
       </c>
       <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
         <v>-989.21394837205116</v>
       </c>
-      <c r="AA9" s="3">
-        <v>0</v>
-      </c>
       <c r="AB9" s="3">
         <v>0</v>
       </c>
       <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
         <v>-887.70944819490865</v>
       </c>
-      <c r="AD9" s="3">
-        <v>0</v>
-      </c>
       <c r="AE9" s="3">
         <v>0</v>
       </c>
       <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
         <v>-796.97075391664043</v>
       </c>
-      <c r="AG9" s="3">
-        <v>0</v>
-      </c>
       <c r="AH9" s="3">
         <v>0</v>
       </c>
       <c r="AI9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="3">
         <v>-715.76055114107919</v>
       </c>
-      <c r="AJ9" s="3">
-        <v>0</v>
-      </c>
       <c r="AK9" s="3">
         <v>0</v>
       </c>
       <c r="AL9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="3">
         <v>-643.16297729171379</v>
       </c>
-      <c r="AM9" s="3">
-        <v>0</v>
-      </c>
       <c r="AN9" s="3">
         <v>0</v>
       </c>
       <c r="AO9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="3">
         <v>-578.14594308184928</v>
       </c>
-      <c r="AP9" s="3">
-        <v>0</v>
-      </c>
       <c r="AQ9" s="3">
         <v>0</v>
       </c>
       <c r="AR9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="3">
         <v>-514.21020439099971</v>
       </c>
-      <c r="AS9" s="3">
-        <v>0</v>
-      </c>
       <c r="AT9" s="3">
         <v>0</v>
       </c>
       <c r="AU9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="3">
         <v>-447.52622922857421</v>
       </c>
-      <c r="AV9" s="3">
-        <v>0</v>
-      </c>
       <c r="AW9" s="3">
         <v>0</v>
       </c>
       <c r="AX9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="3">
         <v>-377.43031433438631</v>
       </c>
-      <c r="AY9" s="3">
-        <v>0</v>
-      </c>
       <c r="AZ9" s="3">
         <v>0</v>
       </c>
       <c r="BA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="3">
         <v>-311.14322108830936</v>
       </c>
-      <c r="BB9" s="3">
-        <v>0</v>
-      </c>
       <c r="BC9" s="3">
         <v>0</v>
       </c>
       <c r="BD9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="3">
         <v>-221.75414952256722</v>
       </c>
-      <c r="BE9" s="3">
-        <v>0</v>
-      </c>
       <c r="BF9" s="3">
         <v>0</v>
       </c>
       <c r="BG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="3">
         <v>-149.14518180503313</v>
       </c>
-      <c r="BH9" s="3">
-        <v>0</v>
-      </c>
       <c r="BI9" s="3">
         <v>0</v>
       </c>
       <c r="BJ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="3">
         <v>-90.491507554494788</v>
       </c>
-      <c r="BK9" s="3">
-        <v>0</v>
-      </c>
       <c r="BL9" s="3">
         <v>0</v>
       </c>
       <c r="BM9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="3">
         <v>-47.475045860823556</v>
       </c>
-      <c r="BN9" s="1"/>
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
       <c r="BQ9" s="1"/>
@@ -3389,9 +3396,9 @@
       <c r="BS9" s="1"/>
       <c r="BT9" s="1"/>
       <c r="BU9" s="1"/>
-    </row>
-    <row r="17" spans="5:25" x14ac:dyDescent="0.35">
-      <c r="E17" s="4"/>
+      <c r="BV9" s="1"/>
+    </row>
+    <row r="17" spans="6:26" x14ac:dyDescent="0.35">
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -3412,6 +3419,7 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3425,7 +3433,7 @@
     <dataValidation type="list" allowBlank="1" sqref="C2:C9" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>VariableType_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:E9" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>Novelty_SystemName</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
revisions for signs + new overview
</commit_message>
<xml_diff>
--- a/PresentValueSeries/CF_CH_2021_12.xlsx
+++ b/PresentValueSeries/CF_CH_2021_12.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39869210-F43E-4495-BAE7-54453A6509FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF737FE-C895-4338-866B-702776940D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="13460" windowHeight="6570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -365,12 +365,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,14 +1493,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.8203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.8203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.8203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -1541,24 +1540,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59E8FC3-4B20-424B-A44D-77DCF1F6F0A1}">
-  <dimension ref="A1:BV17"/>
+  <dimension ref="A1:BV9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" customWidth="1"/>
-    <col min="6" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="66" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.64453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.87890625" customWidth="1"/>
+    <col min="6" max="15" width="10.05859375" bestFit="1" customWidth="1"/>
+    <col min="16" max="66" width="11.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -1772,187 +1771,187 @@
         <v>30</v>
       </c>
       <c r="F2" s="3">
-        <v>80</v>
+        <v>-62.993724880000002</v>
       </c>
       <c r="G2" s="3">
-        <v>80.079999999999984</v>
+        <v>-63.05671860487999</v>
       </c>
       <c r="H2" s="3">
-        <v>80.240159999999989</v>
+        <v>-63.182832042089757</v>
       </c>
       <c r="I2" s="3">
-        <v>80.480880479999982</v>
+        <v>-63.372380538216021</v>
       </c>
       <c r="J2" s="3">
-        <v>80.802804001919981</v>
+        <v>-63.625870060368882</v>
       </c>
       <c r="K2" s="3">
-        <v>81.206818021929578</v>
+        <v>-63.943999410670727</v>
       </c>
       <c r="L2" s="3">
-        <v>81.694058930061161</v>
+        <v>-64.32766340713475</v>
       </c>
       <c r="M2" s="3">
-        <v>82.265917342571584</v>
+        <v>-64.777957050984696</v>
       </c>
       <c r="N2" s="3">
-        <v>82.924044681312154</v>
+        <v>-65.296180707392566</v>
       </c>
       <c r="O2" s="3">
-        <v>83.67036108344395</v>
+        <v>-65.883846333759095</v>
       </c>
       <c r="P2" s="3">
-        <v>84.507064694278384</v>
+        <v>-66.542684797096683</v>
       </c>
       <c r="Q2" s="3">
-        <v>85.521149470609728</v>
+        <v>-67.341197014661844</v>
       </c>
       <c r="R2" s="3">
-        <v>86.718445563198259</v>
+        <v>-68.2839737728671</v>
       </c>
       <c r="S2" s="3">
-        <v>88.10594069220943</v>
+        <v>-69.37651735323297</v>
       </c>
       <c r="T2" s="3">
-        <v>89.691847624669194</v>
+        <v>-70.62529466559117</v>
       </c>
       <c r="U2" s="3">
-        <v>91.485684577162573</v>
+        <v>-72.037800558902987</v>
       </c>
       <c r="V2" s="3">
-        <v>93.498369637860151</v>
+        <v>-73.622632171198845</v>
       </c>
       <c r="W2" s="3">
-        <v>95.742330509168795</v>
+        <v>-75.389575343307627</v>
       </c>
       <c r="X2" s="3">
-        <v>98.423115763425528</v>
+        <v>-77.500483452920236</v>
       </c>
       <c r="Y2" s="3">
-        <v>101.57265546785514</v>
+        <v>-79.980498923413691</v>
       </c>
       <c r="Z2" s="3">
-        <v>105.22927106469793</v>
+        <v>-82.859796884656575</v>
       </c>
       <c r="AA2" s="3">
-        <v>109.43844190728585</v>
+        <v>-86.174188760042853</v>
       </c>
       <c r="AB2" s="3">
-        <v>114.25373335120644</v>
+        <v>-89.965853065484737</v>
       </c>
       <c r="AC2" s="3">
-        <v>119.73791255206434</v>
+        <v>-94.284214012627999</v>
       </c>
       <c r="AD2" s="3">
-        <v>125.9642840047717</v>
+        <v>-99.186993141284674</v>
       </c>
       <c r="AE2" s="3">
-        <v>133.01828390903893</v>
+        <v>-104.74146475719662</v>
       </c>
       <c r="AF2" s="3">
-        <v>141.13239922749028</v>
+        <v>-111.13069410738559</v>
       </c>
       <c r="AG2" s="3">
-        <v>150.44713757650464</v>
+        <v>-118.46531991847306</v>
       </c>
       <c r="AH2" s="3">
-        <v>161.12888434443647</v>
+        <v>-126.87635763268463</v>
       </c>
       <c r="AI2" s="3">
-        <v>173.37467955461366</v>
+        <v>-136.51896081276868</v>
       </c>
       <c r="AJ2" s="3">
-        <v>187.41802859853738</v>
+        <v>-147.57699663860296</v>
       </c>
       <c r="AK2" s="3">
-        <v>203.53597905801161</v>
+        <v>-160.26861834952282</v>
       </c>
       <c r="AL2" s="3">
-        <v>222.05775315229064</v>
+        <v>-174.85306261932939</v>
       </c>
       <c r="AM2" s="3">
-        <v>243.37529745491057</v>
+        <v>-191.638956630785</v>
       </c>
       <c r="AN2" s="3">
-        <v>266.2525754156722</v>
+        <v>-209.65301855407884</v>
       </c>
       <c r="AO2" s="3">
-        <v>290.48155977849837</v>
+        <v>-228.73144324250001</v>
       </c>
       <c r="AP2" s="3">
-        <v>315.75345547922774</v>
+        <v>-248.63107880459754</v>
       </c>
       <c r="AQ2" s="3">
-        <v>341.96099228400362</v>
+        <v>-269.26745834537911</v>
       </c>
       <c r="AR2" s="3">
-        <v>368.97591067443989</v>
+        <v>-290.53958755466402</v>
       </c>
       <c r="AS2" s="3">
-        <v>396.28012806434845</v>
+        <v>-312.03951703370916</v>
       </c>
       <c r="AT2" s="3">
-        <v>423.62345690078848</v>
+        <v>-333.57024370903508</v>
       </c>
       <c r="AU2" s="3">
-        <v>450.735358142439</v>
+        <v>-354.91873930641339</v>
       </c>
       <c r="AV2" s="3">
-        <v>476.8780089147005</v>
+        <v>-375.5040261861854</v>
       </c>
       <c r="AW2" s="3">
-        <v>501.67566537826497</v>
+        <v>-395.03023554786711</v>
       </c>
       <c r="AX2" s="3">
-        <v>523.74939465490866</v>
+        <v>-412.41156591197324</v>
       </c>
       <c r="AY2" s="3">
-        <v>542.08062346783038</v>
+        <v>-426.84597071889226</v>
       </c>
       <c r="AZ2" s="3">
-        <v>555.0905584310583</v>
+        <v>-437.09027401614566</v>
       </c>
       <c r="BA2" s="3">
-        <v>561.75164513223103</v>
+        <v>-442.33535730433942</v>
       </c>
       <c r="BB2" s="3">
-        <v>563.43690006762768</v>
+        <v>-443.66236337625242</v>
       </c>
       <c r="BC2" s="3">
-        <v>560.05627866722193</v>
+        <v>-441.0003891959949</v>
       </c>
       <c r="BD2" s="3">
-        <v>546.61492797920857</v>
+        <v>-430.41637985529104</v>
       </c>
       <c r="BE2" s="3">
-        <v>510.53834273258076</v>
+        <v>-402.00889878484179</v>
       </c>
       <c r="BF2" s="3">
-        <v>463.56881520118333</v>
+        <v>-365.02408009663634</v>
       </c>
       <c r="BG2" s="3">
-        <v>407.01341974663899</v>
+        <v>-320.49114232484669</v>
       </c>
       <c r="BH2" s="3">
-        <v>343.11231284641667</v>
+        <v>-270.17403297984578</v>
       </c>
       <c r="BI2" s="3">
-        <v>275.51918721567256</v>
+        <v>-216.94974848281615</v>
       </c>
       <c r="BJ2" s="3">
-        <v>207.46594797340143</v>
+        <v>-163.36316060756056</v>
       </c>
       <c r="BK2" s="3">
-        <v>143.77390194556719</v>
+        <v>-113.21067030103946</v>
       </c>
       <c r="BL2" s="3">
-        <v>89.571140912088353</v>
+        <v>-70.530247597547586</v>
       </c>
       <c r="BM2" s="3">
-        <v>46.576993274285947</v>
+        <v>-36.675728750724744</v>
       </c>
       <c r="BN2" s="3">
-        <v>13.973097982285781</v>
+        <v>-11.002718625217421</v>
       </c>
       <c r="BO2" s="1"/>
       <c r="BP2" s="1"/>
@@ -1963,7 +1962,7 @@
       <c r="BU2" s="1"/>
       <c r="BV2" s="1"/>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1977,187 +1976,187 @@
         <v>30</v>
       </c>
       <c r="F3" s="3">
-        <v>73.600000000000009</v>
+        <v>-57.954226889600008</v>
       </c>
       <c r="G3" s="3">
-        <v>73.804183056030055</v>
+        <v>-58.115005030308943</v>
       </c>
       <c r="H3" s="3">
-        <v>74.005988873511555</v>
+        <v>-58.273911282129106</v>
       </c>
       <c r="I3" s="3">
-        <v>74.269718768748874</v>
+        <v>-58.481577887919237</v>
       </c>
       <c r="J3" s="3">
-        <v>74.602103085421973</v>
+        <v>-58.743304465405892</v>
       </c>
       <c r="K3" s="3">
-        <v>75.006373842903812</v>
+        <v>-59.061635976328894</v>
       </c>
       <c r="L3" s="3">
-        <v>75.484843073551531</v>
+        <v>-59.438392964815989</v>
       </c>
       <c r="M3" s="3">
-        <v>76.039564981379542</v>
+        <v>-59.875192955398816</v>
       </c>
       <c r="N3" s="3">
-        <v>76.672583056089877</v>
+        <v>-60.373645035928448</v>
       </c>
       <c r="O3" s="3">
-        <v>77.386045313005297</v>
+        <v>-60.935440599983366</v>
       </c>
       <c r="P3" s="3">
-        <v>78.182267965644314</v>
+        <v>-61.562403484027946</v>
       </c>
       <c r="Q3" s="3">
-        <v>79.162546254399487</v>
+        <v>-62.334295744373954</v>
       </c>
       <c r="R3" s="3">
-        <v>80.310070532763987</v>
+        <v>-63.237881102929123</v>
       </c>
       <c r="S3" s="3">
-        <v>81.632147903865302</v>
+        <v>-64.278913330244492</v>
       </c>
       <c r="T3" s="3">
-        <v>83.137014389372965</v>
+        <v>-65.463877647359524</v>
       </c>
       <c r="U3" s="3">
-        <v>84.833991199275289</v>
+        <v>-66.800113775993609</v>
       </c>
       <c r="V3" s="3">
-        <v>86.733618778901089</v>
+        <v>-68.295921490061218</v>
       </c>
       <c r="W3" s="3">
-        <v>88.847787214432557</v>
+        <v>-69.960663299784329</v>
       </c>
       <c r="X3" s="3">
-        <v>91.398523020198041</v>
+        <v>-71.969167669658788</v>
       </c>
       <c r="Y3" s="3">
-        <v>94.38378902608703</v>
+        <v>-74.319830488016123</v>
       </c>
       <c r="Z3" s="3">
-        <v>97.84048680705294</v>
+        <v>-77.041708850609538</v>
       </c>
       <c r="AA3" s="3">
-        <v>101.81202532505596</v>
+        <v>-80.168983910027094</v>
       </c>
       <c r="AB3" s="3">
-        <v>106.34926686943705</v>
+        <v>-83.741705729537699</v>
       </c>
       <c r="AC3" s="3">
-        <v>111.51162183060511</v>
+        <v>-87.806655331496756</v>
       </c>
       <c r="AD3" s="3">
-        <v>117.36833499037918</v>
+        <v>-92.418357550095308</v>
       </c>
       <c r="AE3" s="3">
-        <v>124.00000655936267</v>
+        <v>-97.640278728983603</v>
       </c>
       <c r="AF3" s="3">
-        <v>131.63924730391071</v>
+        <v>-103.65558160091042</v>
       </c>
       <c r="AG3" s="3">
-        <v>140.40441871180292</v>
+        <v>-110.55746655334546</v>
       </c>
       <c r="AH3" s="3">
-        <v>150.45251100323148</v>
+        <v>-118.46955107053421</v>
       </c>
       <c r="AI3" s="3">
-        <v>161.96935505694907</v>
+        <v>-127.53816239310609</v>
       </c>
       <c r="AJ3" s="3">
-        <v>175.17511790862838</v>
+        <v>-137.93666479197122</v>
       </c>
       <c r="AK3" s="3">
-        <v>190.33099133776699</v>
+        <v>-149.87072630586198</v>
       </c>
       <c r="AL3" s="3">
-        <v>207.74734818051408</v>
+        <v>-163.58474119791092</v>
       </c>
       <c r="AM3" s="3">
-        <v>227.79370894463409</v>
+        <v>-179.36967788316346</v>
       </c>
       <c r="AN3" s="3">
-        <v>249.16177239767649</v>
+        <v>-196.19535176290515</v>
       </c>
       <c r="AO3" s="3">
-        <v>271.76161553762893</v>
+        <v>-213.99095552652165</v>
       </c>
       <c r="AP3" s="3">
-        <v>295.29571363611007</v>
+        <v>-232.52221178795477</v>
       </c>
       <c r="AQ3" s="3">
-        <v>319.68428445689688</v>
+        <v>-251.7262982942178</v>
       </c>
       <c r="AR3" s="3">
-        <v>344.80562754757858</v>
+        <v>-271.50738548509895</v>
       </c>
       <c r="AS3" s="3">
-        <v>370.13651614737176</v>
+        <v>-291.4534733278652</v>
       </c>
       <c r="AT3" s="3">
-        <v>395.47166973057449</v>
+        <v>-311.40291951052541</v>
       </c>
       <c r="AU3" s="3">
-        <v>420.55648958365617</v>
+        <v>-331.15524751664282</v>
       </c>
       <c r="AV3" s="3">
-        <v>444.64998164767547</v>
+        <v>-350.12698264763401</v>
       </c>
       <c r="AW3" s="3">
-        <v>467.44073541042076</v>
+        <v>-368.07291355186152</v>
       </c>
       <c r="AX3" s="3">
-        <v>487.51460902938481</v>
+        <v>-383.87951445222291</v>
       </c>
       <c r="AY3" s="3">
-        <v>503.94367963936435</v>
+        <v>-396.8161188777122</v>
       </c>
       <c r="AZ3" s="3">
-        <v>515.11768679476836</v>
+        <v>-405.61477303464562</v>
       </c>
       <c r="BA3" s="3">
-        <v>519.98471567021829</v>
+        <v>-409.44717650918449</v>
       </c>
       <c r="BB3" s="3">
-        <v>519.95330893972323</v>
+        <v>-409.42244617243216</v>
       </c>
       <c r="BC3" s="3">
-        <v>517.48879736462914</v>
+        <v>-407.48183662086899</v>
       </c>
       <c r="BD3" s="3">
-        <v>507.25239871488412</v>
+        <v>-399.4214756170685</v>
       </c>
       <c r="BE3" s="3">
-        <v>476.45864451893556</v>
+        <v>-375.17380961904433</v>
       </c>
       <c r="BF3" s="3">
-        <v>433.73385895599188</v>
+        <v>-341.53139227768099</v>
       </c>
       <c r="BG3" s="3">
-        <v>381.78314678385362</v>
+        <v>-300.62428140403415</v>
       </c>
       <c r="BH3" s="3">
-        <v>322.67382619765033</v>
+        <v>-254.08032791839653</v>
       </c>
       <c r="BI3" s="3">
-        <v>259.78356161859261</v>
+        <v>-204.55917761185191</v>
       </c>
       <c r="BJ3" s="3">
-        <v>196.18556690700947</v>
+        <v>-154.48074533958734</v>
       </c>
       <c r="BK3" s="3">
-        <v>136.3798155198939</v>
+        <v>-107.38840722556688</v>
       </c>
       <c r="BL3" s="3">
-        <v>85.241419067552911</v>
+        <v>-67.120931264027675</v>
       </c>
       <c r="BM3" s="3">
-        <v>44.514839598436339</v>
+        <v>-35.051944484265356</v>
       </c>
       <c r="BN3" s="3">
-        <v>13.458093512555834</v>
+        <v>-10.597193001740688</v>
       </c>
       <c r="BO3" s="1"/>
       <c r="BP3" s="1"/>
@@ -2168,7 +2167,7 @@
       <c r="BU3" s="1"/>
       <c r="BV3" s="1"/>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
@@ -2182,187 +2181,187 @@
         <v>30</v>
       </c>
       <c r="F4" s="3">
-        <v>80</v>
+        <v>-62.993724880000002</v>
       </c>
       <c r="G4" s="3">
-        <v>80.221938104380499</v>
+        <v>-63.168483728596676</v>
       </c>
       <c r="H4" s="3">
-        <v>80.441292253816911</v>
+        <v>-63.341207915357721</v>
       </c>
       <c r="I4" s="3">
-        <v>80.727955183422679</v>
+        <v>-63.56693248686873</v>
       </c>
       <c r="J4" s="3">
-        <v>81.089242484154312</v>
+        <v>-63.851417897180312</v>
       </c>
       <c r="K4" s="3">
-        <v>81.528667220547618</v>
+        <v>-64.19743040905314</v>
       </c>
       <c r="L4" s="3">
-        <v>82.048742471251657</v>
+        <v>-64.606948874799983</v>
       </c>
       <c r="M4" s="3">
-        <v>82.651701066716882</v>
+        <v>-65.08173147325958</v>
       </c>
       <c r="N4" s="3">
-        <v>83.33976419140204</v>
+        <v>-65.623527212965698</v>
       </c>
       <c r="O4" s="3">
-        <v>84.115266644570966</v>
+        <v>-66.234174565199311</v>
       </c>
       <c r="P4" s="3">
-        <v>84.980726049613381</v>
+        <v>-66.91565596089994</v>
       </c>
       <c r="Q4" s="3">
-        <v>86.046245928695086</v>
+        <v>-67.754669287362987</v>
       </c>
       <c r="R4" s="3">
-        <v>87.293554926917366</v>
+        <v>-68.736827285792515</v>
       </c>
       <c r="S4" s="3">
-        <v>88.73059554767967</v>
+        <v>-69.868384054613585</v>
       </c>
       <c r="T4" s="3">
-        <v>90.366319988448865</v>
+        <v>-71.15638874712991</v>
       </c>
       <c r="U4" s="3">
-        <v>92.210859999212261</v>
+        <v>-72.608819321732184</v>
       </c>
       <c r="V4" s="3">
-        <v>94.275672585762052</v>
+        <v>-74.234697271805672</v>
       </c>
       <c r="W4" s="3">
-        <v>96.573681754817997</v>
+        <v>-76.044199238896013</v>
       </c>
       <c r="X4" s="3">
-        <v>99.346220674128304</v>
+        <v>-78.227356162672592</v>
       </c>
       <c r="Y4" s="3">
-        <v>102.59107502835546</v>
+        <v>-80.782424443495785</v>
       </c>
       <c r="Z4" s="3">
-        <v>106.34835522505755</v>
+        <v>-83.740987881097325</v>
       </c>
       <c r="AA4" s="3">
-        <v>110.66524491853907</v>
+        <v>-87.140199902203364</v>
       </c>
       <c r="AB4" s="3">
-        <v>115.59702920590982</v>
+        <v>-91.023593184280102</v>
       </c>
       <c r="AC4" s="3">
-        <v>121.2082845984838</v>
+        <v>-95.442016664670376</v>
       </c>
       <c r="AD4" s="3">
-        <v>127.57427716345563</v>
+        <v>-100.4547364674949</v>
       </c>
       <c r="AE4" s="3">
-        <v>134.7826158253942</v>
+        <v>-106.13073774889521</v>
       </c>
       <c r="AF4" s="3">
-        <v>143.08613837381597</v>
+        <v>-112.66911043577218</v>
       </c>
       <c r="AG4" s="3">
-        <v>152.61349859978577</v>
+        <v>-120.17115929711463</v>
       </c>
       <c r="AH4" s="3">
-        <v>163.53533804699072</v>
+        <v>-128.77125116362413</v>
       </c>
       <c r="AI4" s="3">
-        <v>176.05364680103159</v>
+        <v>-138.62843738381096</v>
       </c>
       <c r="AJ4" s="3">
-        <v>190.40773685720475</v>
+        <v>-149.9311573825774</v>
       </c>
       <c r="AK4" s="3">
-        <v>206.88151232365976</v>
+        <v>-162.90296337593691</v>
       </c>
       <c r="AL4" s="3">
-        <v>225.81233497881965</v>
+        <v>-177.80950130207708</v>
       </c>
       <c r="AM4" s="3">
-        <v>247.60185754851531</v>
+        <v>-194.96704117735158</v>
       </c>
       <c r="AN4" s="3">
-        <v>270.8280134757353</v>
+        <v>-213.25581713359253</v>
       </c>
       <c r="AO4" s="3">
-        <v>295.39306036698792</v>
+        <v>-232.59886470274088</v>
       </c>
       <c r="AP4" s="3">
-        <v>320.9736017783805</v>
+        <v>-252.74153455212476</v>
       </c>
       <c r="AQ4" s="3">
-        <v>347.48291788793136</v>
+        <v>-273.61554162414973</v>
       </c>
       <c r="AR4" s="3">
-        <v>374.78872559519408</v>
+        <v>-295.1167233533684</v>
       </c>
       <c r="AS4" s="3">
-        <v>402.32230016018667</v>
+        <v>-316.79725361724473</v>
       </c>
       <c r="AT4" s="3">
-        <v>429.86051057671136</v>
+        <v>-338.48143425057111</v>
       </c>
       <c r="AU4" s="3">
-        <v>457.12661911266974</v>
+        <v>-359.95135599635086</v>
       </c>
       <c r="AV4" s="3">
-        <v>483.3151974431255</v>
+        <v>-380.57280722568913</v>
       </c>
       <c r="AW4" s="3">
-        <v>508.08775588089208</v>
+        <v>-400.07925386071901</v>
       </c>
       <c r="AX4" s="3">
-        <v>529.90718372759216</v>
+        <v>-417.26034179589442</v>
       </c>
       <c r="AY4" s="3">
-        <v>547.76486917322211</v>
+        <v>-431.32186834533934</v>
       </c>
       <c r="AZ4" s="3">
-        <v>559.91052912474822</v>
+        <v>-440.88562286374525</v>
       </c>
       <c r="BA4" s="3">
-        <v>565.20077790241112</v>
+        <v>-445.05127881433089</v>
       </c>
       <c r="BB4" s="3">
-        <v>565.16664015187303</v>
+        <v>-445.02439801351318</v>
       </c>
       <c r="BC4" s="3">
-        <v>562.487823222423</v>
+        <v>-442.91503980529239</v>
       </c>
       <c r="BD4" s="3">
-        <v>551.36130295096098</v>
+        <v>-434.15377784463965</v>
       </c>
       <c r="BE4" s="3">
-        <v>517.88983099884297</v>
+        <v>-407.79761915113517</v>
       </c>
       <c r="BF4" s="3">
-        <v>471.44984669129548</v>
+        <v>-371.22977421487059</v>
       </c>
       <c r="BG4" s="3">
-        <v>414.98168128679742</v>
+        <v>-326.76552326525456</v>
       </c>
       <c r="BH4" s="3">
-        <v>350.73241978005467</v>
+        <v>-276.17426947651796</v>
       </c>
       <c r="BI4" s="3">
-        <v>282.37343654194848</v>
+        <v>-222.34693218679553</v>
       </c>
       <c r="BJ4" s="3">
-        <v>213.24518142066248</v>
+        <v>-167.91385362998625</v>
       </c>
       <c r="BK4" s="3">
-        <v>148.23892991292814</v>
+        <v>-116.72652959300748</v>
       </c>
       <c r="BL4" s="3">
-        <v>92.653716377774899</v>
+        <v>-72.957533982638779</v>
       </c>
       <c r="BM4" s="3">
-        <v>48.385695215691669</v>
+        <v>-38.099939656810172</v>
       </c>
       <c r="BN4" s="3">
-        <v>14.628362513647645</v>
+        <v>-11.518688045370313</v>
       </c>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
@@ -2373,7 +2372,7 @@
       <c r="BU4" s="1"/>
       <c r="BV4" s="1"/>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
@@ -2387,187 +2386,187 @@
         <v>40</v>
       </c>
       <c r="F5" s="3">
-        <v>80</v>
+        <v>-62.993724880000002</v>
       </c>
       <c r="G5" s="3">
-        <v>80.221938104380499</v>
+        <v>-63.168483728596676</v>
       </c>
       <c r="H5" s="3">
-        <v>80.441292253816911</v>
+        <v>-63.341207915357721</v>
       </c>
       <c r="I5" s="3">
-        <v>80.727955183422679</v>
+        <v>-63.56693248686873</v>
       </c>
       <c r="J5" s="3">
-        <v>81.089242484154312</v>
+        <v>-63.851417897180312</v>
       </c>
       <c r="K5" s="3">
-        <v>81.528667220547618</v>
+        <v>-64.19743040905314</v>
       </c>
       <c r="L5" s="3">
-        <v>82.048742471251657</v>
+        <v>-64.606948874799983</v>
       </c>
       <c r="M5" s="3">
-        <v>82.651701066716882</v>
+        <v>-65.08173147325958</v>
       </c>
       <c r="N5" s="3">
-        <v>83.33976419140204</v>
+        <v>-65.623527212965698</v>
       </c>
       <c r="O5" s="3">
-        <v>84.115266644570966</v>
+        <v>-66.234174565199311</v>
       </c>
       <c r="P5" s="3">
-        <v>84.980726049613381</v>
+        <v>-66.91565596089994</v>
       </c>
       <c r="Q5" s="3">
-        <v>86.046245928695086</v>
+        <v>-67.754669287362987</v>
       </c>
       <c r="R5" s="3">
-        <v>87.293554926917366</v>
+        <v>-68.736827285792515</v>
       </c>
       <c r="S5" s="3">
-        <v>88.73059554767967</v>
+        <v>-69.868384054613585</v>
       </c>
       <c r="T5" s="3">
-        <v>90.366319988448865</v>
+        <v>-71.15638874712991</v>
       </c>
       <c r="U5" s="3">
-        <v>92.210859999212261</v>
+        <v>-72.608819321732184</v>
       </c>
       <c r="V5" s="3">
-        <v>94.275672585762052</v>
+        <v>-74.234697271805672</v>
       </c>
       <c r="W5" s="3">
-        <v>96.573681754817997</v>
+        <v>-76.044199238896013</v>
       </c>
       <c r="X5" s="3">
-        <v>99.346220674128304</v>
+        <v>-78.227356162672592</v>
       </c>
       <c r="Y5" s="3">
-        <v>102.59107502835546</v>
+        <v>-80.782424443495785</v>
       </c>
       <c r="Z5" s="3">
-        <v>106.34835522505755</v>
+        <v>-83.740987881097325</v>
       </c>
       <c r="AA5" s="3">
-        <v>110.66524491853907</v>
+        <v>-87.140199902203364</v>
       </c>
       <c r="AB5" s="3">
-        <v>115.59702920590982</v>
+        <v>-91.023593184280102</v>
       </c>
       <c r="AC5" s="3">
-        <v>121.2082845984838</v>
+        <v>-95.442016664670376</v>
       </c>
       <c r="AD5" s="3">
-        <v>127.57427716345563</v>
+        <v>-100.4547364674949</v>
       </c>
       <c r="AE5" s="3">
-        <v>134.7826158253942</v>
+        <v>-106.13073774889521</v>
       </c>
       <c r="AF5" s="3">
-        <v>143.08613837381597</v>
+        <v>-112.66911043577218</v>
       </c>
       <c r="AG5" s="3">
-        <v>152.61349859978577</v>
+        <v>-120.17115929711463</v>
       </c>
       <c r="AH5" s="3">
-        <v>163.53533804699072</v>
+        <v>-128.77125116362413</v>
       </c>
       <c r="AI5" s="3">
-        <v>176.05364680103159</v>
+        <v>-138.62843738381096</v>
       </c>
       <c r="AJ5" s="3">
-        <v>190.40773685720475</v>
+        <v>-149.9311573825774</v>
       </c>
       <c r="AK5" s="3">
-        <v>206.88151232365976</v>
+        <v>-162.90296337593691</v>
       </c>
       <c r="AL5" s="3">
-        <v>225.81233497881965</v>
+        <v>-177.80950130207708</v>
       </c>
       <c r="AM5" s="3">
-        <v>247.60185754851531</v>
+        <v>-194.96704117735158</v>
       </c>
       <c r="AN5" s="3">
-        <v>270.8280134757353</v>
+        <v>-213.25581713359253</v>
       </c>
       <c r="AO5" s="3">
-        <v>295.39306036698792</v>
+        <v>-232.59886470274088</v>
       </c>
       <c r="AP5" s="3">
-        <v>320.9736017783805</v>
+        <v>-252.74153455212476</v>
       </c>
       <c r="AQ5" s="3">
-        <v>347.48291788793136</v>
+        <v>-273.61554162414973</v>
       </c>
       <c r="AR5" s="3">
-        <v>374.78872559519408</v>
+        <v>-295.1167233533684</v>
       </c>
       <c r="AS5" s="3">
-        <v>402.32230016018667</v>
+        <v>-316.79725361724473</v>
       </c>
       <c r="AT5" s="3">
-        <v>429.86051057671136</v>
+        <v>-338.48143425057111</v>
       </c>
       <c r="AU5" s="3">
-        <v>457.12661911266974</v>
+        <v>-359.95135599635086</v>
       </c>
       <c r="AV5" s="3">
-        <v>483.3151974431255</v>
+        <v>-380.57280722568913</v>
       </c>
       <c r="AW5" s="3">
-        <v>508.08775588089208</v>
+        <v>-400.07925386071901</v>
       </c>
       <c r="AX5" s="3">
-        <v>529.90718372759216</v>
+        <v>-417.26034179589442</v>
       </c>
       <c r="AY5" s="3">
-        <v>547.76486917322211</v>
+        <v>-431.32186834533934</v>
       </c>
       <c r="AZ5" s="3">
-        <v>559.91052912474822</v>
+        <v>-440.88562286374525</v>
       </c>
       <c r="BA5" s="3">
-        <v>565.20077790241112</v>
+        <v>-445.05127881433089</v>
       </c>
       <c r="BB5" s="3">
-        <v>565.16664015187303</v>
+        <v>-445.02439801351318</v>
       </c>
       <c r="BC5" s="3">
-        <v>562.487823222423</v>
+        <v>-442.91503980529239</v>
       </c>
       <c r="BD5" s="3">
-        <v>551.36130295096098</v>
+        <v>-434.15377784463965</v>
       </c>
       <c r="BE5" s="3">
-        <v>517.88983099884297</v>
+        <v>-407.79761915113517</v>
       </c>
       <c r="BF5" s="3">
-        <v>471.44984669129548</v>
+        <v>-371.22977421487059</v>
       </c>
       <c r="BG5" s="3">
-        <v>414.98168128679742</v>
+        <v>-326.76552326525456</v>
       </c>
       <c r="BH5" s="3">
-        <v>350.73241978005467</v>
+        <v>-276.17426947651796</v>
       </c>
       <c r="BI5" s="3">
-        <v>282.37343654194848</v>
+        <v>-222.34693218679553</v>
       </c>
       <c r="BJ5" s="3">
-        <v>213.24518142066248</v>
+        <v>-167.91385362998625</v>
       </c>
       <c r="BK5" s="3">
-        <v>148.23892991292814</v>
+        <v>-116.72652959300748</v>
       </c>
       <c r="BL5" s="3">
-        <v>92.653716377774899</v>
+        <v>-72.957533982638779</v>
       </c>
       <c r="BM5" s="3">
-        <v>48.385695215691669</v>
+        <v>-38.099939656810172</v>
       </c>
       <c r="BN5" s="3">
-        <v>14.628362513647645</v>
+        <v>-11.518688045370313</v>
       </c>
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
@@ -2578,7 +2577,7 @@
       <c r="BU5" s="1"/>
       <c r="BV5" s="1"/>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="3">
-        <v>-2210.5500000000002</v>
+        <v>1740.6347316685503</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2601,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="3">
-        <v>-1989.4950000000001</v>
+        <v>1566.5712585016952</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -2610,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="3">
-        <v>-1790.5455000000002</v>
+        <v>1409.9141326515257</v>
       </c>
       <c r="M6" s="3">
         <v>0</v>
@@ -2619,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="3">
-        <v>-1611.4909500000001</v>
+        <v>1268.922719386373</v>
       </c>
       <c r="P6" s="3">
         <v>0</v>
@@ -2628,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="3">
-        <v>-1450.3418550000001</v>
+        <v>1142.0304474477359</v>
       </c>
       <c r="S6" s="3">
         <v>0</v>
@@ -2637,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="3">
-        <v>-1305.3076695000002</v>
+        <v>1027.8274027029622</v>
       </c>
       <c r="V6" s="3">
         <v>0</v>
@@ -2646,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="3">
-        <v>-1174.7769025500002</v>
+        <v>925.04466243266609</v>
       </c>
       <c r="Y6" s="3">
         <v>0</v>
@@ -2655,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="3">
-        <v>-1057.2992122950002</v>
+        <v>832.54019618939947</v>
       </c>
       <c r="AB6" s="3">
         <v>0</v>
@@ -2664,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="AD6" s="3">
-        <v>-951.56929106550024</v>
+        <v>749.28617657045959</v>
       </c>
       <c r="AE6" s="3">
         <v>0</v>
@@ -2673,7 +2672,7 @@
         <v>0</v>
       </c>
       <c r="AG6" s="3">
-        <v>-856.41236195895021</v>
+        <v>674.35755891341364</v>
       </c>
       <c r="AH6" s="3">
         <v>0</v>
@@ -2682,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="3">
-        <v>-770.77112576305524</v>
+        <v>606.92180302207225</v>
       </c>
       <c r="AK6" s="3">
         <v>0</v>
@@ -2691,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="AM6" s="3">
-        <v>-693.69401318674977</v>
+        <v>546.22962271986512</v>
       </c>
       <c r="AN6" s="3">
         <v>0</v>
@@ -2700,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="AP6" s="3">
-        <v>-624.32461186807484</v>
+        <v>491.60666044787865</v>
       </c>
       <c r="AQ6" s="3">
         <v>0</v>
@@ -2709,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="AS6" s="3">
-        <v>-555.64890456258661</v>
+        <v>437.52992779861199</v>
       </c>
       <c r="AT6" s="3">
         <v>0</v>
@@ -2718,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="AV6" s="3">
-        <v>-483.41454696945033</v>
+        <v>380.65103718479241</v>
       </c>
       <c r="AW6" s="3">
         <v>0</v>
@@ -2727,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="AY6" s="3">
-        <v>-406.06821945433825</v>
+        <v>319.74687123522563</v>
       </c>
       <c r="AZ6" s="3">
         <v>0</v>
@@ -2736,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="BB6" s="3">
-        <v>-324.85457556347063</v>
+        <v>255.79749698818051</v>
       </c>
       <c r="BC6" s="3">
         <v>0</v>
@@ -2745,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="BE6" s="3">
-        <v>-243.64093167260296</v>
+        <v>191.84812274113537</v>
       </c>
       <c r="BF6" s="3">
         <v>0</v>
@@ -2754,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="BH6" s="3">
-        <v>-168.11224285409602</v>
+        <v>132.3752046913834</v>
       </c>
       <c r="BI6" s="3">
         <v>0</v>
@@ -2763,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="BK6" s="3">
-        <v>-104.22959056953954</v>
+        <v>82.07262690865771</v>
       </c>
       <c r="BL6" s="3">
         <v>0</v>
@@ -2772,7 +2771,7 @@
         <v>0</v>
       </c>
       <c r="BN6" s="3">
-        <v>-56.283978907551358</v>
+        <v>44.319218530675165</v>
       </c>
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
@@ -2783,7 +2782,7 @@
       <c r="BU6" s="1"/>
       <c r="BV6" s="1"/>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>82</v>
       </c>
@@ -2797,7 +2796,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="3">
-        <v>-2210.5500000000002</v>
+        <v>1740.6347316685503</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2806,7 +2805,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="3">
-        <v>-2063.2215160144488</v>
+        <v>1624.6251068288839</v>
       </c>
       <c r="J7" s="3">
         <v>0</v>
@@ -2815,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="3">
-        <v>-1882.8080036188367</v>
+        <v>1482.5636172728382</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
@@ -2824,7 +2823,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <v>-1709.2914496442083</v>
+        <v>1345.9329414827955</v>
       </c>
       <c r="P7" s="3">
         <v>0</v>
@@ -2833,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="3">
-        <v>-1548.107757870913</v>
+        <v>1219.0134272989244</v>
       </c>
       <c r="S7" s="3">
         <v>0</v>
@@ -2842,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="U7" s="3">
-        <v>-1400.2266747581864</v>
+        <v>1102.5686739919304</v>
       </c>
       <c r="V7" s="3">
         <v>0</v>
@@ -2851,7 +2850,7 @@
         <v>0</v>
       </c>
       <c r="X7" s="3">
-        <v>-1265.3600787277182</v>
+        <v>996.37180841886288</v>
       </c>
       <c r="Y7" s="3">
         <v>0</v>
@@ -2860,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="AA7" s="3">
-        <v>-1142.6680434267498</v>
+        <v>899.76145445990721</v>
       </c>
       <c r="AB7" s="3">
         <v>0</v>
@@ -2869,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="AD7" s="3">
-        <v>-1031.1590303291489</v>
+        <v>811.95685330102481</v>
       </c>
       <c r="AE7" s="3">
         <v>0</v>
@@ -2878,7 +2877,7 @@
         <v>0</v>
       </c>
       <c r="AG7" s="3">
-        <v>-930.12425790876898</v>
+        <v>732.39989508648955</v>
       </c>
       <c r="AH7" s="3">
         <v>0</v>
@@ -2887,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="3">
-        <v>-838.69960468102829</v>
+        <v>660.41015192801819</v>
       </c>
       <c r="AK7" s="3">
         <v>0</v>
@@ -2896,7 +2895,7 @@
         <v>0</v>
       </c>
       <c r="AM7" s="3">
-        <v>-755.89487156573273</v>
+        <v>595.20791972018378</v>
       </c>
       <c r="AN7" s="3">
         <v>0</v>
@@ -2905,7 +2904,7 @@
         <v>0</v>
       </c>
       <c r="AP7" s="3">
-        <v>-681.03269727904706</v>
+        <v>536.25982958350767</v>
       </c>
       <c r="AQ7" s="3">
         <v>0</v>
@@ -2914,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="AS7" s="3">
-        <v>-606.47057787820472</v>
+        <v>477.54800913342808</v>
       </c>
       <c r="AT7" s="3">
         <v>0</v>
@@ -2923,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="AV7" s="3">
-        <v>-527.46046281648682</v>
+        <v>415.33374099674052</v>
       </c>
       <c r="AW7" s="3">
         <v>0</v>
@@ -2932,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="AY7" s="3">
-        <v>-441.49550282763306</v>
+        <v>347.64307801101478</v>
       </c>
       <c r="AZ7" s="3">
         <v>0</v>
@@ -2941,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="BB7" s="3">
-        <v>-342.98899321869982</v>
+        <v>270.07692844608704</v>
       </c>
       <c r="BC7" s="3">
         <v>0</v>
@@ -2950,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="BE7" s="3">
-        <v>-269.66796579728577</v>
+        <v>212.3423705797934</v>
       </c>
       <c r="BF7" s="3">
         <v>0</v>
@@ -2959,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="3">
-        <v>-189.73508154216125</v>
+        <v>149.40149408439092</v>
       </c>
       <c r="BI7" s="3">
         <v>0</v>
@@ -2968,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="3">
-        <v>-119.40335697364351</v>
+        <v>94.020777736826616</v>
       </c>
       <c r="BL7" s="3">
         <v>0</v>
@@ -2977,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="BN7" s="3">
-        <v>-65.653826382205708</v>
+        <v>51.697238455499402</v>
       </c>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
@@ -2988,7 +2987,7 @@
       <c r="BU7" s="1"/>
       <c r="BV7" s="1"/>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>82</v>
       </c>
@@ -3002,7 +3001,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="3">
-        <v>-2210.5500000000002</v>
+        <v>1740.6347316685503</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3011,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="3">
-        <v>-1936.0518028052484</v>
+        <v>1524.4889327417729</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
@@ -3020,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="3">
-        <v>-1721.4454032739382</v>
+        <v>1355.503226622239</v>
       </c>
       <c r="M8" s="3">
         <v>0</v>
@@ -3029,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="3">
-        <v>-1536.7528388427074</v>
+        <v>1210.0723192327061</v>
       </c>
       <c r="P8" s="3">
         <v>0</v>
@@ -3038,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="3">
-        <v>-1374.5375449647067</v>
+        <v>1082.3404993092172</v>
       </c>
       <c r="S8" s="3">
         <v>0</v>
@@ -3047,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="3">
-        <v>-1230.8726159976718</v>
+        <v>969.21563668104034</v>
       </c>
       <c r="V8" s="3">
         <v>0</v>
@@ -3056,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="3">
-        <v>-1103.0807329563593</v>
+        <v>868.58955265352063</v>
       </c>
       <c r="Y8" s="3">
         <v>0</v>
@@ -3065,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="3">
-        <v>-989.21394837205116</v>
+        <v>778.92839139009402</v>
       </c>
       <c r="AB8" s="3">
         <v>0</v>
@@ -3074,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="AD8" s="3">
-        <v>-887.70944819490865</v>
+        <v>699.00155941208368</v>
       </c>
       <c r="AE8" s="3">
         <v>0</v>
@@ -3083,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="AG8" s="3">
-        <v>-796.97075391664043</v>
+        <v>627.5519551203879</v>
       </c>
       <c r="AH8" s="3">
         <v>0</v>
@@ -3092,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="3">
-        <v>-715.76055114107919</v>
+        <v>563.60529048172896</v>
       </c>
       <c r="AK8" s="3">
         <v>0</v>
@@ -3101,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="AM8" s="3">
-        <v>-643.16297729171379</v>
+        <v>506.44039555644883</v>
       </c>
       <c r="AN8" s="3">
         <v>0</v>
@@ -3110,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="AP8" s="3">
-        <v>-578.14594308184928</v>
+        <v>455.24458098732691</v>
       </c>
       <c r="AQ8" s="3">
         <v>0</v>
@@ -3119,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="AS8" s="3">
-        <v>-514.21020439099971</v>
+        <v>404.90020182369005</v>
       </c>
       <c r="AT8" s="3">
         <v>0</v>
@@ -3128,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="AV8" s="3">
-        <v>-447.52622922857421</v>
+        <v>352.39180200760774</v>
       </c>
       <c r="AW8" s="3">
         <v>0</v>
@@ -3137,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="AY8" s="3">
-        <v>-377.43031433438631</v>
+        <v>297.19676728190313</v>
       </c>
       <c r="AZ8" s="3">
         <v>0</v>
@@ -3146,7 +3145,7 @@
         <v>0</v>
       </c>
       <c r="BB8" s="3">
-        <v>-311.14322108830936</v>
+        <v>245.00088084392468</v>
       </c>
       <c r="BC8" s="3">
         <v>0</v>
@@ -3155,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="BE8" s="3">
-        <v>-221.75414952256722</v>
+        <v>174.6139985752873</v>
       </c>
       <c r="BF8" s="3">
         <v>0</v>
@@ -3164,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="3">
-        <v>-149.14518180503313</v>
+        <v>117.44013187254799</v>
       </c>
       <c r="BI8" s="3">
         <v>0</v>
@@ -3173,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="3">
-        <v>-90.491507554494788</v>
+        <v>71.25496413580359</v>
       </c>
       <c r="BL8" s="3">
         <v>0</v>
@@ -3182,7 +3181,7 @@
         <v>0</v>
       </c>
       <c r="BN8" s="3">
-        <v>-47.475045860823556</v>
+        <v>37.382874720276277</v>
       </c>
       <c r="BO8" s="1"/>
       <c r="BP8" s="1"/>
@@ -3193,7 +3192,7 @@
       <c r="BU8" s="1"/>
       <c r="BV8" s="1"/>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="3">
-        <v>-2210.5500000000002</v>
+        <v>1740.6347316685503</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -3216,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="3">
-        <v>-1936.0518028052484</v>
+        <v>1524.4889327417729</v>
       </c>
       <c r="J9" s="3">
         <v>0</v>
@@ -3225,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>-1721.4454032739382</v>
+        <v>1355.503226622239</v>
       </c>
       <c r="M9" s="3">
         <v>0</v>
@@ -3234,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="3">
-        <v>-1536.7528388427074</v>
+        <v>1210.0723192327061</v>
       </c>
       <c r="P9" s="3">
         <v>0</v>
@@ -3243,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="3">
-        <v>-1374.5375449647067</v>
+        <v>1082.3404993092172</v>
       </c>
       <c r="S9" s="3">
         <v>0</v>
@@ -3252,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="U9" s="3">
-        <v>-1230.8726159976718</v>
+        <v>969.21563668104034</v>
       </c>
       <c r="V9" s="3">
         <v>0</v>
@@ -3261,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="3">
-        <v>-1103.0807329563593</v>
+        <v>868.58955265352063</v>
       </c>
       <c r="Y9" s="3">
         <v>0</v>
@@ -3270,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="3">
-        <v>-989.21394837205116</v>
+        <v>778.92839139009402</v>
       </c>
       <c r="AB9" s="3">
         <v>0</v>
@@ -3279,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="AD9" s="3">
-        <v>-887.70944819490865</v>
+        <v>699.00155941208368</v>
       </c>
       <c r="AE9" s="3">
         <v>0</v>
@@ -3288,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="AG9" s="3">
-        <v>-796.97075391664043</v>
+        <v>627.5519551203879</v>
       </c>
       <c r="AH9" s="3">
         <v>0</v>
@@ -3297,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="3">
-        <v>-715.76055114107919</v>
+        <v>563.60529048172896</v>
       </c>
       <c r="AK9" s="3">
         <v>0</v>
@@ -3306,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="AM9" s="3">
-        <v>-643.16297729171379</v>
+        <v>506.44039555644883</v>
       </c>
       <c r="AN9" s="3">
         <v>0</v>
@@ -3315,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="AP9" s="3">
-        <v>-578.14594308184928</v>
+        <v>455.24458098732691</v>
       </c>
       <c r="AQ9" s="3">
         <v>0</v>
@@ -3324,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="AS9" s="3">
-        <v>-514.21020439099971</v>
+        <v>404.90020182369005</v>
       </c>
       <c r="AT9" s="3">
         <v>0</v>
@@ -3333,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="AV9" s="3">
-        <v>-447.52622922857421</v>
+        <v>352.39180200760774</v>
       </c>
       <c r="AW9" s="3">
         <v>0</v>
@@ -3342,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="AY9" s="3">
-        <v>-377.43031433438631</v>
+        <v>297.19676728190313</v>
       </c>
       <c r="AZ9" s="3">
         <v>0</v>
@@ -3351,7 +3350,7 @@
         <v>0</v>
       </c>
       <c r="BB9" s="3">
-        <v>-311.14322108830936</v>
+        <v>245.00088084392468</v>
       </c>
       <c r="BC9" s="3">
         <v>0</v>
@@ -3360,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="BE9" s="3">
-        <v>-221.75414952256722</v>
+        <v>174.6139985752873</v>
       </c>
       <c r="BF9" s="3">
         <v>0</v>
@@ -3369,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="BH9" s="3">
-        <v>-149.14518180503313</v>
+        <v>117.44013187254799</v>
       </c>
       <c r="BI9" s="3">
         <v>0</v>
@@ -3378,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="BK9" s="3">
-        <v>-90.491507554494788</v>
+        <v>71.25496413580359</v>
       </c>
       <c r="BL9" s="3">
         <v>0</v>
@@ -3387,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="BN9" s="3">
-        <v>-47.475045860823556</v>
+        <v>37.382874720276277</v>
       </c>
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
@@ -3397,29 +3396,6 @@
       <c r="BT9" s="1"/>
       <c r="BU9" s="1"/>
       <c r="BV9" s="1"/>
-    </row>
-    <row r="17" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3454,7 +3430,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -3463,7 +3439,7 @@
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3483,7 +3459,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -3503,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -3523,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -3537,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -3551,7 +3527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -3562,7 +3538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -3570,7 +3546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -3578,7 +3554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -3586,7 +3562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -3594,7 +3570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -3602,7 +3578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -3610,7 +3586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -3618,457 +3594,457 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>1982</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>1983</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>1984</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>1985</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>1986</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>1987</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>1988</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>1989</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>1990</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>1991</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>1992</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>1993</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>1994</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>1995</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>1996</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>1997</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>1998</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>1999</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>2001</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>2002</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>2003</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>2004</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>2006</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>2007</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>2008</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>2009</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>2010</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>2011</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>2012</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>2014</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>2015</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>2016</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>2018</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>2019</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>2020</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>2021</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>2022</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>2023</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>2024</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>2025</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>2026</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>2027</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>2028</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>2029</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>2030</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>2031</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>2032</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>2033</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>2034</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>2035</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>2036</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>2037</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>2038</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>2039</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>2040</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>2041</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>2042</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>2043</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>2044</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>2045</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>2046</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>2047</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>2048</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>2049</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>2050</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>2051</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>2052</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>2053</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>2054</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>2055</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>2056</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>2057</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>2058</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>2059</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>2060</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>2061</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>2062</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>2063</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>2064</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>2065</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>2066</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>2067</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>2068</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>2069</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>2070</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>2071</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>2072</v>
       </c>

</xml_diff>

<commit_message>
pv update xlsx files
</commit_message>
<xml_diff>
--- a/PresentValueSeries/CF_CH_2021_12.xlsx
+++ b/PresentValueSeries/CF_CH_2021_12.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79592C8D-7BE4-413D-A5F6-498990AC447A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA158AB5-65C1-4113-BF5D-21E052E62050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
   <si>
     <t>ReportingNode</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>GIC1_CH</t>
+  </si>
+  <si>
+    <t>EstimateType</t>
+  </si>
+  <si>
+    <t>BE</t>
   </si>
 </sst>
 </file>
@@ -362,9 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1113,11 +1117,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BM9" totalsRowShown="0">
-  <autoFilter ref="A1:BM9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BN9" totalsRowShown="0">
+  <autoFilter ref="A1:BN9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="66">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DataNode" dataDxfId="64"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="AmountType" dataDxfId="63"/>
+    <tableColumn id="66" xr3:uid="{AF8EC0ED-2C9B-4356-9792-12C929510FE4}" name="EstimateType"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="AocType" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Novelty" dataDxfId="61"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Values0" dataDxfId="60"/>
@@ -1536,23 +1541,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59E8FC3-4B20-424B-A44D-77DCF1F6F0A1}">
-  <dimension ref="A1:BU9"/>
+  <dimension ref="A1:BV9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.3515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.87890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="10.05859375" bestFit="1" customWidth="1"/>
-    <col min="15" max="65" width="11.05859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3515625" customWidth="1"/>
+    <col min="4" max="4" width="10.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="10.05859375" bestFit="1" customWidth="1"/>
+    <col min="16" max="66" width="11.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1560,392 +1566,397 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>51</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>53</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>54</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>56</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>57</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>58</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>59</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>60</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>61</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>62</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>63</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>64</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>65</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>66</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>67</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>68</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>69</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>70</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>71</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>72</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>73</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>74</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>75</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>76</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>77</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>78</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>79</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="1">
         <v>-62.993724880000002</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="1">
         <v>-63.05671860487999</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="1">
         <v>-63.182832042089757</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="1">
         <v>-63.372380538216021</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="1">
         <v>-63.625870060368882</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="1">
         <v>-63.943999410670727</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="1">
         <v>-64.32766340713475</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="1">
         <v>-64.777957050984696</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="1">
         <v>-65.296180707392566</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="1">
         <v>-65.883846333759095</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="1">
         <v>-66.542684797096683</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="1">
         <v>-67.341197014661844</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="1">
         <v>-68.2839737728671</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="1">
         <v>-69.37651735323297</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="1">
         <v>-70.62529466559117</v>
       </c>
-      <c r="T2" s="3">
+      <c r="U2" s="1">
         <v>-72.037800558902987</v>
       </c>
-      <c r="U2" s="3">
+      <c r="V2" s="1">
         <v>-73.622632171198845</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="1">
         <v>-75.389575343307627</v>
       </c>
-      <c r="W2" s="3">
+      <c r="X2" s="1">
         <v>-77.500483452920236</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Y2" s="1">
         <v>-79.980498923413691</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Z2" s="1">
         <v>-82.859796884656575</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="1">
         <v>-86.174188760042853</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AB2" s="1">
         <v>-89.965853065484737</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AC2" s="1">
         <v>-94.284214012627999</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AD2" s="1">
         <v>-99.186993141284674</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AE2" s="1">
         <v>-104.74146475719662</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AF2" s="1">
         <v>-111.13069410738559</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AG2" s="1">
         <v>-118.46531991847306</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AH2" s="1">
         <v>-126.87635763268463</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AI2" s="1">
         <v>-136.51896081276868</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AJ2" s="1">
         <v>-147.57699663860296</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AK2" s="1">
         <v>-160.26861834952282</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AL2" s="1">
         <v>-174.85306261932939</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AM2" s="1">
         <v>-191.638956630785</v>
       </c>
-      <c r="AM2" s="3">
+      <c r="AN2" s="1">
         <v>-209.65301855407884</v>
       </c>
-      <c r="AN2" s="3">
+      <c r="AO2" s="1">
         <v>-228.73144324250001</v>
       </c>
-      <c r="AO2" s="3">
+      <c r="AP2" s="1">
         <v>-248.63107880459754</v>
       </c>
-      <c r="AP2" s="3">
+      <c r="AQ2" s="1">
         <v>-269.26745834537911</v>
       </c>
-      <c r="AQ2" s="3">
+      <c r="AR2" s="1">
         <v>-290.53958755466402</v>
       </c>
-      <c r="AR2" s="3">
+      <c r="AS2" s="1">
         <v>-312.03951703370916</v>
       </c>
-      <c r="AS2" s="3">
+      <c r="AT2" s="1">
         <v>-333.57024370903508</v>
       </c>
-      <c r="AT2" s="3">
+      <c r="AU2" s="1">
         <v>-354.91873930641339</v>
       </c>
-      <c r="AU2" s="3">
+      <c r="AV2" s="1">
         <v>-375.5040261861854</v>
       </c>
-      <c r="AV2" s="3">
+      <c r="AW2" s="1">
         <v>-395.03023554786711</v>
       </c>
-      <c r="AW2" s="3">
+      <c r="AX2" s="1">
         <v>-412.41156591197324</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="AY2" s="1">
         <v>-426.84597071889226</v>
       </c>
-      <c r="AY2" s="3">
+      <c r="AZ2" s="1">
         <v>-437.09027401614566</v>
       </c>
-      <c r="AZ2" s="3">
+      <c r="BA2" s="1">
         <v>-442.33535730433942</v>
       </c>
-      <c r="BA2" s="3">
+      <c r="BB2" s="1">
         <v>-443.66236337625242</v>
       </c>
-      <c r="BB2" s="3">
+      <c r="BC2" s="1">
         <v>-441.0003891959949</v>
       </c>
-      <c r="BC2" s="3">
+      <c r="BD2" s="1">
         <v>-430.41637985529104</v>
       </c>
-      <c r="BD2" s="3">
+      <c r="BE2" s="1">
         <v>-402.00889878484179</v>
       </c>
-      <c r="BE2" s="3">
+      <c r="BF2" s="1">
         <v>-365.02408009663634</v>
       </c>
-      <c r="BF2" s="3">
+      <c r="BG2" s="1">
         <v>-320.49114232484669</v>
       </c>
-      <c r="BG2" s="3">
+      <c r="BH2" s="1">
         <v>-270.17403297984578</v>
       </c>
-      <c r="BH2" s="3">
+      <c r="BI2" s="1">
         <v>-216.94974848281615</v>
       </c>
-      <c r="BI2" s="3">
+      <c r="BJ2" s="1">
         <v>-163.36316060756056</v>
       </c>
-      <c r="BJ2" s="3">
+      <c r="BK2" s="1">
         <v>-113.21067030103946</v>
       </c>
-      <c r="BK2" s="3">
+      <c r="BL2" s="1">
         <v>-70.530247597547586</v>
       </c>
-      <c r="BL2" s="3">
+      <c r="BM2" s="1">
         <v>-36.675728750724744</v>
       </c>
-      <c r="BM2" s="3">
+      <c r="BN2" s="1">
         <v>-11.002718625217421</v>
       </c>
-      <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1"/>
@@ -1953,204 +1964,207 @@
       <c r="BS2" s="1"/>
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
-    </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
+      <c r="BV2" s="1"/>
+    </row>
+    <row r="3" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
       <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="1">
         <v>-57.954226889600008</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="1">
         <v>-58.115005030308943</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="1">
         <v>-58.273911282129106</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="1">
         <v>-58.481577887919237</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="1">
         <v>-58.743304465405892</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="1">
         <v>-59.061635976328894</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="1">
         <v>-59.438392964815989</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="1">
         <v>-59.875192955398816</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="1">
         <v>-60.373645035928448</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="1">
         <v>-60.935440599983366</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="1">
         <v>-61.562403484027946</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="1">
         <v>-62.334295744373954</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="1">
         <v>-63.237881102929123</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="1">
         <v>-64.278913330244492</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="1">
         <v>-65.463877647359524</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="1">
         <v>-66.800113775993609</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="1">
         <v>-68.295921490061218</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="1">
         <v>-69.960663299784329</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="1">
         <v>-71.969167669658788</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="1">
         <v>-74.319830488016123</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="1">
         <v>-77.041708850609538</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="1">
         <v>-80.168983910027094</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="1">
         <v>-83.741705729537699</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="1">
         <v>-87.806655331496756</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="1">
         <v>-92.418357550095308</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="1">
         <v>-97.640278728983603</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="1">
         <v>-103.65558160091042</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="1">
         <v>-110.55746655334546</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AH3" s="1">
         <v>-118.46955107053421</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AI3" s="1">
         <v>-127.53816239310609</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AJ3" s="1">
         <v>-137.93666479197122</v>
       </c>
-      <c r="AJ3" s="3">
+      <c r="AK3" s="1">
         <v>-149.87072630586198</v>
       </c>
-      <c r="AK3" s="3">
+      <c r="AL3" s="1">
         <v>-163.58474119791092</v>
       </c>
-      <c r="AL3" s="3">
+      <c r="AM3" s="1">
         <v>-179.36967788316346</v>
       </c>
-      <c r="AM3" s="3">
+      <c r="AN3" s="1">
         <v>-196.19535176290515</v>
       </c>
-      <c r="AN3" s="3">
+      <c r="AO3" s="1">
         <v>-213.99095552652165</v>
       </c>
-      <c r="AO3" s="3">
+      <c r="AP3" s="1">
         <v>-232.52221178795477</v>
       </c>
-      <c r="AP3" s="3">
+      <c r="AQ3" s="1">
         <v>-251.7262982942178</v>
       </c>
-      <c r="AQ3" s="3">
+      <c r="AR3" s="1">
         <v>-271.50738548509895</v>
       </c>
-      <c r="AR3" s="3">
+      <c r="AS3" s="1">
         <v>-291.4534733278652</v>
       </c>
-      <c r="AS3" s="3">
+      <c r="AT3" s="1">
         <v>-311.40291951052541</v>
       </c>
-      <c r="AT3" s="3">
+      <c r="AU3" s="1">
         <v>-331.15524751664282</v>
       </c>
-      <c r="AU3" s="3">
+      <c r="AV3" s="1">
         <v>-350.12698264763401</v>
       </c>
-      <c r="AV3" s="3">
+      <c r="AW3" s="1">
         <v>-368.07291355186152</v>
       </c>
-      <c r="AW3" s="3">
+      <c r="AX3" s="1">
         <v>-383.87951445222291</v>
       </c>
-      <c r="AX3" s="3">
+      <c r="AY3" s="1">
         <v>-396.8161188777122</v>
       </c>
-      <c r="AY3" s="3">
+      <c r="AZ3" s="1">
         <v>-405.61477303464562</v>
       </c>
-      <c r="AZ3" s="3">
+      <c r="BA3" s="1">
         <v>-409.44717650918449</v>
       </c>
-      <c r="BA3" s="3">
+      <c r="BB3" s="1">
         <v>-409.42244617243216</v>
       </c>
-      <c r="BB3" s="3">
+      <c r="BC3" s="1">
         <v>-407.48183662086899</v>
       </c>
-      <c r="BC3" s="3">
+      <c r="BD3" s="1">
         <v>-399.4214756170685</v>
       </c>
-      <c r="BD3" s="3">
+      <c r="BE3" s="1">
         <v>-375.17380961904433</v>
       </c>
-      <c r="BE3" s="3">
+      <c r="BF3" s="1">
         <v>-341.53139227768099</v>
       </c>
-      <c r="BF3" s="3">
+      <c r="BG3" s="1">
         <v>-300.62428140403415</v>
       </c>
-      <c r="BG3" s="3">
+      <c r="BH3" s="1">
         <v>-254.08032791839653</v>
       </c>
-      <c r="BH3" s="3">
+      <c r="BI3" s="1">
         <v>-204.55917761185191</v>
       </c>
-      <c r="BI3" s="3">
+      <c r="BJ3" s="1">
         <v>-154.48074533958734</v>
       </c>
-      <c r="BJ3" s="3">
+      <c r="BK3" s="1">
         <v>-107.38840722556688</v>
       </c>
-      <c r="BK3" s="3">
+      <c r="BL3" s="1">
         <v>-67.120931264027675</v>
       </c>
-      <c r="BL3" s="3">
+      <c r="BM3" s="1">
         <v>-35.051944484265356</v>
       </c>
-      <c r="BM3" s="3">
+      <c r="BN3" s="1">
         <v>-10.597193001740688</v>
       </c>
-      <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
@@ -2158,204 +2172,207 @@
       <c r="BS3" s="1"/>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
-    </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
+      <c r="BV3" s="1"/>
+    </row>
+    <row r="4" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="1">
         <v>-62.993724880000002</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="1">
         <v>-63.168483728596676</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="1">
         <v>-63.341207915357721</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="1">
         <v>-63.56693248686873</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="1">
         <v>-63.851417897180312</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="1">
         <v>-64.19743040905314</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="1">
         <v>-64.606948874799983</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="1">
         <v>-65.08173147325958</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="1">
         <v>-65.623527212965698</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="1">
         <v>-66.234174565199311</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="1">
         <v>-66.91565596089994</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="1">
         <v>-67.754669287362987</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="1">
         <v>-68.736827285792515</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="1">
         <v>-69.868384054613585</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="1">
         <v>-71.15638874712991</v>
       </c>
-      <c r="T4" s="3">
+      <c r="U4" s="1">
         <v>-72.608819321732184</v>
       </c>
-      <c r="U4" s="3">
+      <c r="V4" s="1">
         <v>-74.234697271805672</v>
       </c>
-      <c r="V4" s="3">
+      <c r="W4" s="1">
         <v>-76.044199238896013</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="1">
         <v>-78.227356162672592</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Y4" s="1">
         <v>-80.782424443495785</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Z4" s="1">
         <v>-83.740987881097325</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AA4" s="1">
         <v>-87.140199902203364</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="1">
         <v>-91.023593184280102</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AC4" s="1">
         <v>-95.442016664670376</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AD4" s="1">
         <v>-100.4547364674949</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AE4" s="1">
         <v>-106.13073774889521</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AF4" s="1">
         <v>-112.66911043577218</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AG4" s="1">
         <v>-120.17115929711463</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AH4" s="1">
         <v>-128.77125116362413</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AI4" s="1">
         <v>-138.62843738381096</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AJ4" s="1">
         <v>-149.9311573825774</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AK4" s="1">
         <v>-162.90296337593691</v>
       </c>
-      <c r="AK4" s="3">
+      <c r="AL4" s="1">
         <v>-177.80950130207708</v>
       </c>
-      <c r="AL4" s="3">
+      <c r="AM4" s="1">
         <v>-194.96704117735158</v>
       </c>
-      <c r="AM4" s="3">
+      <c r="AN4" s="1">
         <v>-213.25581713359253</v>
       </c>
-      <c r="AN4" s="3">
+      <c r="AO4" s="1">
         <v>-232.59886470274088</v>
       </c>
-      <c r="AO4" s="3">
+      <c r="AP4" s="1">
         <v>-252.74153455212476</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AQ4" s="1">
         <v>-273.61554162414973</v>
       </c>
-      <c r="AQ4" s="3">
+      <c r="AR4" s="1">
         <v>-295.1167233533684</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AS4" s="1">
         <v>-316.79725361724473</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AT4" s="1">
         <v>-338.48143425057111</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AU4" s="1">
         <v>-359.95135599635086</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AV4" s="1">
         <v>-380.57280722568913</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AW4" s="1">
         <v>-400.07925386071901</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AX4" s="1">
         <v>-417.26034179589442</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AY4" s="1">
         <v>-431.32186834533934</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AZ4" s="1">
         <v>-440.88562286374525</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="BA4" s="1">
         <v>-445.05127881433089</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BB4" s="1">
         <v>-445.02439801351318</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BC4" s="1">
         <v>-442.91503980529239</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BD4" s="1">
         <v>-434.15377784463965</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BE4" s="1">
         <v>-407.79761915113517</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BF4" s="1">
         <v>-371.22977421487059</v>
       </c>
-      <c r="BF4" s="3">
+      <c r="BG4" s="1">
         <v>-326.76552326525456</v>
       </c>
-      <c r="BG4" s="3">
+      <c r="BH4" s="1">
         <v>-276.17426947651796</v>
       </c>
-      <c r="BH4" s="3">
+      <c r="BI4" s="1">
         <v>-222.34693218679553</v>
       </c>
-      <c r="BI4" s="3">
+      <c r="BJ4" s="1">
         <v>-167.91385362998625</v>
       </c>
-      <c r="BJ4" s="3">
+      <c r="BK4" s="1">
         <v>-116.72652959300748</v>
       </c>
-      <c r="BK4" s="3">
+      <c r="BL4" s="1">
         <v>-72.957533982638779</v>
       </c>
-      <c r="BL4" s="3">
+      <c r="BM4" s="1">
         <v>-38.099939656810172</v>
       </c>
-      <c r="BM4" s="3">
+      <c r="BN4" s="1">
         <v>-11.518688045370313</v>
       </c>
-      <c r="BN4" s="1"/>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
@@ -2363,204 +2380,207 @@
       <c r="BS4" s="1"/>
       <c r="BT4" s="1"/>
       <c r="BU4" s="1"/>
-    </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
+      <c r="BV4" s="1"/>
+    </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="1">
         <v>-62.993724880000002</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="1">
         <v>-63.168483728596676</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="1">
         <v>-63.341207915357721</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="1">
         <v>-63.56693248686873</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="1">
         <v>-63.851417897180312</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="1">
         <v>-64.19743040905314</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="1">
         <v>-64.606948874799983</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="1">
         <v>-65.08173147325958</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="1">
         <v>-65.623527212965698</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="1">
         <v>-66.234174565199311</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="1">
         <v>-66.91565596089994</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="1">
         <v>-67.754669287362987</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="1">
         <v>-68.736827285792515</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="1">
         <v>-69.868384054613585</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="1">
         <v>-71.15638874712991</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="1">
         <v>-72.608819321732184</v>
       </c>
-      <c r="U5" s="3">
+      <c r="V5" s="1">
         <v>-74.234697271805672</v>
       </c>
-      <c r="V5" s="3">
+      <c r="W5" s="1">
         <v>-76.044199238896013</v>
       </c>
-      <c r="W5" s="3">
+      <c r="X5" s="1">
         <v>-78.227356162672592</v>
       </c>
-      <c r="X5" s="3">
+      <c r="Y5" s="1">
         <v>-80.782424443495785</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Z5" s="1">
         <v>-83.740987881097325</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="AA5" s="1">
         <v>-87.140199902203364</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AB5" s="1">
         <v>-91.023593184280102</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AC5" s="1">
         <v>-95.442016664670376</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="AD5" s="1">
         <v>-100.4547364674949</v>
       </c>
-      <c r="AD5" s="3">
+      <c r="AE5" s="1">
         <v>-106.13073774889521</v>
       </c>
-      <c r="AE5" s="3">
+      <c r="AF5" s="1">
         <v>-112.66911043577218</v>
       </c>
-      <c r="AF5" s="3">
+      <c r="AG5" s="1">
         <v>-120.17115929711463</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AH5" s="1">
         <v>-128.77125116362413</v>
       </c>
-      <c r="AH5" s="3">
+      <c r="AI5" s="1">
         <v>-138.62843738381096</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AJ5" s="1">
         <v>-149.9311573825774</v>
       </c>
-      <c r="AJ5" s="3">
+      <c r="AK5" s="1">
         <v>-162.90296337593691</v>
       </c>
-      <c r="AK5" s="3">
+      <c r="AL5" s="1">
         <v>-177.80950130207708</v>
       </c>
-      <c r="AL5" s="3">
+      <c r="AM5" s="1">
         <v>-194.96704117735158</v>
       </c>
-      <c r="AM5" s="3">
+      <c r="AN5" s="1">
         <v>-213.25581713359253</v>
       </c>
-      <c r="AN5" s="3">
+      <c r="AO5" s="1">
         <v>-232.59886470274088</v>
       </c>
-      <c r="AO5" s="3">
+      <c r="AP5" s="1">
         <v>-252.74153455212476</v>
       </c>
-      <c r="AP5" s="3">
+      <c r="AQ5" s="1">
         <v>-273.61554162414973</v>
       </c>
-      <c r="AQ5" s="3">
+      <c r="AR5" s="1">
         <v>-295.1167233533684</v>
       </c>
-      <c r="AR5" s="3">
+      <c r="AS5" s="1">
         <v>-316.79725361724473</v>
       </c>
-      <c r="AS5" s="3">
+      <c r="AT5" s="1">
         <v>-338.48143425057111</v>
       </c>
-      <c r="AT5" s="3">
+      <c r="AU5" s="1">
         <v>-359.95135599635086</v>
       </c>
-      <c r="AU5" s="3">
+      <c r="AV5" s="1">
         <v>-380.57280722568913</v>
       </c>
-      <c r="AV5" s="3">
+      <c r="AW5" s="1">
         <v>-400.07925386071901</v>
       </c>
-      <c r="AW5" s="3">
+      <c r="AX5" s="1">
         <v>-417.26034179589442</v>
       </c>
-      <c r="AX5" s="3">
+      <c r="AY5" s="1">
         <v>-431.32186834533934</v>
       </c>
-      <c r="AY5" s="3">
+      <c r="AZ5" s="1">
         <v>-440.88562286374525</v>
       </c>
-      <c r="AZ5" s="3">
+      <c r="BA5" s="1">
         <v>-445.05127881433089</v>
       </c>
-      <c r="BA5" s="3">
+      <c r="BB5" s="1">
         <v>-445.02439801351318</v>
       </c>
-      <c r="BB5" s="3">
+      <c r="BC5" s="1">
         <v>-442.91503980529239</v>
       </c>
-      <c r="BC5" s="3">
+      <c r="BD5" s="1">
         <v>-434.15377784463965</v>
       </c>
-      <c r="BD5" s="3">
+      <c r="BE5" s="1">
         <v>-407.79761915113517</v>
       </c>
-      <c r="BE5" s="3">
+      <c r="BF5" s="1">
         <v>-371.22977421487059</v>
       </c>
-      <c r="BF5" s="3">
+      <c r="BG5" s="1">
         <v>-326.76552326525456</v>
       </c>
-      <c r="BG5" s="3">
+      <c r="BH5" s="1">
         <v>-276.17426947651796</v>
       </c>
-      <c r="BH5" s="3">
+      <c r="BI5" s="1">
         <v>-222.34693218679553</v>
       </c>
-      <c r="BI5" s="3">
+      <c r="BJ5" s="1">
         <v>-167.91385362998625</v>
       </c>
-      <c r="BJ5" s="3">
+      <c r="BK5" s="1">
         <v>-116.72652959300748</v>
       </c>
-      <c r="BK5" s="3">
+      <c r="BL5" s="1">
         <v>-72.957533982638779</v>
       </c>
-      <c r="BL5" s="3">
+      <c r="BM5" s="1">
         <v>-38.099939656810172</v>
       </c>
-      <c r="BM5" s="3">
+      <c r="BN5" s="1">
         <v>-11.518688045370313</v>
       </c>
-      <c r="BN5" s="1"/>
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
@@ -2568,204 +2588,207 @@
       <c r="BS5" s="1"/>
       <c r="BT5" s="1"/>
       <c r="BU5" s="1"/>
-    </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
+      <c r="BV5" s="1"/>
+    </row>
+    <row r="6" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>1566.5712585016952</v>
       </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>1409.9141326515257</v>
       </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
         <v>1268.922719386373</v>
       </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
         <v>1142.0304474477359</v>
       </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3">
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
         <v>1027.8274027029622</v>
       </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
         <v>925.04466243266609</v>
       </c>
-      <c r="X6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="3">
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
         <v>832.54019618939947</v>
       </c>
-      <c r="AA6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="3">
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
         <v>749.28617657045959</v>
       </c>
-      <c r="AD6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="3">
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
         <v>674.35755891341364</v>
       </c>
-      <c r="AG6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="3">
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
         <v>606.92180302207225</v>
       </c>
-      <c r="AJ6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="3">
+      <c r="AK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
         <v>546.22962271986512</v>
       </c>
-      <c r="AM6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="3">
+      <c r="AN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="1">
         <v>491.60666044787865</v>
       </c>
-      <c r="AP6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="3">
+      <c r="AQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="1">
         <v>437.52992779861199</v>
       </c>
-      <c r="AS6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="3">
+      <c r="AT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="1">
         <v>380.65103718479241</v>
       </c>
-      <c r="AV6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="3">
+      <c r="AW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="1">
         <v>319.74687123522563</v>
       </c>
-      <c r="AY6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="3">
+      <c r="AZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="1">
         <v>255.79749698818051</v>
       </c>
-      <c r="BB6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="3">
+      <c r="BC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="1">
         <v>191.84812274113537</v>
       </c>
-      <c r="BE6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG6" s="3">
+      <c r="BF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="1">
         <v>132.3752046913834</v>
       </c>
-      <c r="BH6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="3">
+      <c r="BI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="1">
         <v>82.07262690865771</v>
       </c>
-      <c r="BK6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM6" s="3">
+      <c r="BL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="1">
         <v>44.319218530675165</v>
       </c>
-      <c r="BN6" s="1"/>
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
@@ -2773,204 +2796,207 @@
       <c r="BS6" s="1"/>
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
-    </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A7" s="2" t="s">
+      <c r="BV6" s="1"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
         <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
         <v>1624.6251068288839</v>
       </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>1482.5636172728382</v>
       </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3">
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
         <v>1345.9329414827955</v>
       </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
         <v>1219.0134272989244</v>
       </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
         <v>1102.5686739919304</v>
       </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3">
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
         <v>996.37180841886288</v>
       </c>
-      <c r="X7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="3">
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
         <v>899.76145445990721</v>
       </c>
-      <c r="AA7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="3">
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
         <v>811.95685330102481</v>
       </c>
-      <c r="AD7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3">
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
         <v>732.39989508648955</v>
       </c>
-      <c r="AG7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="3">
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
         <v>660.41015192801819</v>
       </c>
-      <c r="AJ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="3">
+      <c r="AK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
         <v>595.20791972018378</v>
       </c>
-      <c r="AM7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="3">
+      <c r="AN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="1">
         <v>536.25982958350767</v>
       </c>
-      <c r="AP7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="3">
+      <c r="AQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="1">
         <v>477.54800913342808</v>
       </c>
-      <c r="AS7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="3">
+      <c r="AT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="1">
         <v>415.33374099674052</v>
       </c>
-      <c r="AV7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="3">
+      <c r="AW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="1">
         <v>347.64307801101478</v>
       </c>
-      <c r="AY7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="3">
+      <c r="AZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="1">
         <v>270.07692844608704</v>
       </c>
-      <c r="BB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD7" s="3">
+      <c r="BC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
         <v>212.3423705797934</v>
       </c>
-      <c r="BE7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG7" s="3">
+      <c r="BF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="1">
         <v>149.40149408439092</v>
       </c>
-      <c r="BH7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="3">
+      <c r="BI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="1">
         <v>94.020777736826616</v>
       </c>
-      <c r="BK7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM7" s="3">
+      <c r="BL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="1">
         <v>51.697238455499402</v>
       </c>
-      <c r="BN7" s="1"/>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
@@ -2978,204 +3004,207 @@
       <c r="BS7" s="1"/>
       <c r="BT7" s="1"/>
       <c r="BU7" s="1"/>
-    </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A8" s="2" t="s">
+      <c r="BV7" s="1"/>
+    </row>
+    <row r="8" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
         <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
         <v>1524.4889327417729</v>
       </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
         <v>1355.503226622239</v>
       </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3">
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
         <v>1210.0723192327061</v>
       </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
         <v>1082.3404993092172</v>
       </c>
-      <c r="R8" s="3">
-        <v>0</v>
-      </c>
-      <c r="S8" s="3">
-        <v>0</v>
-      </c>
-      <c r="T8" s="3">
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
         <v>969.21563668104034</v>
       </c>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3">
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
         <v>868.58955265352063</v>
       </c>
-      <c r="X8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3">
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
         <v>778.92839139009402</v>
       </c>
-      <c r="AA8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="3">
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
         <v>699.00155941208368</v>
       </c>
-      <c r="AD8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3">
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
         <v>627.5519551203879</v>
       </c>
-      <c r="AG8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="3">
+      <c r="AH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1">
         <v>563.60529048172896</v>
       </c>
-      <c r="AJ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="3">
+      <c r="AK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="1">
         <v>506.44039555644883</v>
       </c>
-      <c r="AM8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="3">
+      <c r="AN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="1">
         <v>455.24458098732691</v>
       </c>
-      <c r="AP8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="3">
+      <c r="AQ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="1">
         <v>404.90020182369005</v>
       </c>
-      <c r="AS8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="3">
+      <c r="AT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1">
         <v>352.39180200760774</v>
       </c>
-      <c r="AV8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="3">
+      <c r="AW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="1">
         <v>297.19676728190313</v>
       </c>
-      <c r="AY8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="3">
+      <c r="AZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="1">
         <v>245.00088084392468</v>
       </c>
-      <c r="BB8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="3">
+      <c r="BC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="1">
         <v>174.6139985752873</v>
       </c>
-      <c r="BE8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="3">
+      <c r="BF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="1">
         <v>117.44013187254799</v>
       </c>
-      <c r="BH8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="3">
+      <c r="BI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="1">
         <v>71.25496413580359</v>
       </c>
-      <c r="BK8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM8" s="3">
+      <c r="BL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="1">
         <v>37.382874720276277</v>
       </c>
-      <c r="BN8" s="1"/>
       <c r="BO8" s="1"/>
       <c r="BP8" s="1"/>
       <c r="BQ8" s="1"/>
@@ -3183,204 +3212,207 @@
       <c r="BS8" s="1"/>
       <c r="BT8" s="1"/>
       <c r="BU8" s="1"/>
-    </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A9" s="2" t="s">
+      <c r="BV8" s="1"/>
+    </row>
+    <row r="9" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
         <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
         <v>1524.4889327417729</v>
       </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>1355.503226622239</v>
       </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
         <v>1210.0723192327061</v>
       </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3">
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
         <v>1082.3404993092172</v>
       </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
-      <c r="T9" s="3">
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
         <v>969.21563668104034</v>
       </c>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
-      <c r="V9" s="3">
-        <v>0</v>
-      </c>
-      <c r="W9" s="3">
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
         <v>868.58955265352063</v>
       </c>
-      <c r="X9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="3">
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
         <v>778.92839139009402</v>
       </c>
-      <c r="AA9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="3">
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
         <v>699.00155941208368</v>
       </c>
-      <c r="AD9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3">
+      <c r="AE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1">
         <v>627.5519551203879</v>
       </c>
-      <c r="AG9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="3">
+      <c r="AH9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1">
         <v>563.60529048172896</v>
       </c>
-      <c r="AJ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="3">
+      <c r="AK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1">
         <v>506.44039555644883</v>
       </c>
-      <c r="AM9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="3">
+      <c r="AN9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1">
         <v>455.24458098732691</v>
       </c>
-      <c r="AP9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="3">
+      <c r="AQ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="1">
         <v>404.90020182369005</v>
       </c>
-      <c r="AS9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="3">
+      <c r="AT9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="1">
         <v>352.39180200760774</v>
       </c>
-      <c r="AV9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="3">
+      <c r="AW9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="1">
         <v>297.19676728190313</v>
       </c>
-      <c r="AY9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="3">
+      <c r="AZ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="1">
         <v>245.00088084392468</v>
       </c>
-      <c r="BB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD9" s="3">
+      <c r="BC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="1">
         <v>174.6139985752873</v>
       </c>
-      <c r="BE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="3">
+      <c r="BF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="1">
         <v>117.44013187254799</v>
       </c>
-      <c r="BH9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="3">
+      <c r="BI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="1">
         <v>71.25496413580359</v>
       </c>
-      <c r="BK9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM9" s="3">
+      <c r="BL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="1">
         <v>37.382874720276277</v>
       </c>
-      <c r="BN9" s="1"/>
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
       <c r="BQ9" s="1"/>
@@ -3388,6 +3420,7 @@
       <c r="BS9" s="1"/>
       <c r="BT9" s="1"/>
       <c r="BU9" s="1"/>
+      <c r="BV9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3395,20 +3428,20 @@
     <dataValidation type="list" allowBlank="1" sqref="A2:A9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>GroupOfContract_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B9" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:C9" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>AmountType_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C9" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>VariableType_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E9" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>Novelty_SystemName</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B6:C6 D3 C2 D2" numberStoredAsText="1" calculatedColumn="1"/>
+    <ignoredError sqref="D6 E3 D2:E2 B6" numberStoredAsText="1" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Cleaning the diff (a bit).
</commit_message>
<xml_diff>
--- a/PresentValueSeries/CF_CH_2021_12.xlsx
+++ b/PresentValueSeries/CF_CH_2021_12.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79592C8D-7BE4-413D-A5F6-498990AC447A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA158AB5-65C1-4113-BF5D-21E052E62050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
   <si>
     <t>ReportingNode</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>GIC1_CH</t>
+  </si>
+  <si>
+    <t>EstimateType</t>
+  </si>
+  <si>
+    <t>BE</t>
   </si>
 </sst>
 </file>
@@ -362,9 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1113,11 +1117,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BM9" totalsRowShown="0">
-  <autoFilter ref="A1:BM9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BN9" totalsRowShown="0">
+  <autoFilter ref="A1:BN9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="66">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DataNode" dataDxfId="64"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="AmountType" dataDxfId="63"/>
+    <tableColumn id="66" xr3:uid="{AF8EC0ED-2C9B-4356-9792-12C929510FE4}" name="EstimateType"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="AocType" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Novelty" dataDxfId="61"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Values0" dataDxfId="60"/>
@@ -1536,23 +1541,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59E8FC3-4B20-424B-A44D-77DCF1F6F0A1}">
-  <dimension ref="A1:BU9"/>
+  <dimension ref="A1:BV9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.3515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.87890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="10.05859375" bestFit="1" customWidth="1"/>
-    <col min="15" max="65" width="11.05859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3515625" customWidth="1"/>
+    <col min="4" max="4" width="10.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="10.05859375" bestFit="1" customWidth="1"/>
+    <col min="16" max="66" width="11.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1560,392 +1566,397 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>51</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>53</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>54</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>56</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>57</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>58</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>59</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>60</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>61</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>62</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>63</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>64</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>65</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>66</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>67</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>68</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>69</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>70</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>71</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>72</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>73</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>74</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>75</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>76</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>77</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>78</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>79</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="1">
         <v>-62.993724880000002</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="1">
         <v>-63.05671860487999</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="1">
         <v>-63.182832042089757</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="1">
         <v>-63.372380538216021</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="1">
         <v>-63.625870060368882</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="1">
         <v>-63.943999410670727</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="1">
         <v>-64.32766340713475</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="1">
         <v>-64.777957050984696</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="1">
         <v>-65.296180707392566</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="1">
         <v>-65.883846333759095</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="1">
         <v>-66.542684797096683</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="1">
         <v>-67.341197014661844</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="1">
         <v>-68.2839737728671</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="1">
         <v>-69.37651735323297</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="1">
         <v>-70.62529466559117</v>
       </c>
-      <c r="T2" s="3">
+      <c r="U2" s="1">
         <v>-72.037800558902987</v>
       </c>
-      <c r="U2" s="3">
+      <c r="V2" s="1">
         <v>-73.622632171198845</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="1">
         <v>-75.389575343307627</v>
       </c>
-      <c r="W2" s="3">
+      <c r="X2" s="1">
         <v>-77.500483452920236</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Y2" s="1">
         <v>-79.980498923413691</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Z2" s="1">
         <v>-82.859796884656575</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="1">
         <v>-86.174188760042853</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AB2" s="1">
         <v>-89.965853065484737</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AC2" s="1">
         <v>-94.284214012627999</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AD2" s="1">
         <v>-99.186993141284674</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AE2" s="1">
         <v>-104.74146475719662</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AF2" s="1">
         <v>-111.13069410738559</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AG2" s="1">
         <v>-118.46531991847306</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AH2" s="1">
         <v>-126.87635763268463</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AI2" s="1">
         <v>-136.51896081276868</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AJ2" s="1">
         <v>-147.57699663860296</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AK2" s="1">
         <v>-160.26861834952282</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AL2" s="1">
         <v>-174.85306261932939</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AM2" s="1">
         <v>-191.638956630785</v>
       </c>
-      <c r="AM2" s="3">
+      <c r="AN2" s="1">
         <v>-209.65301855407884</v>
       </c>
-      <c r="AN2" s="3">
+      <c r="AO2" s="1">
         <v>-228.73144324250001</v>
       </c>
-      <c r="AO2" s="3">
+      <c r="AP2" s="1">
         <v>-248.63107880459754</v>
       </c>
-      <c r="AP2" s="3">
+      <c r="AQ2" s="1">
         <v>-269.26745834537911</v>
       </c>
-      <c r="AQ2" s="3">
+      <c r="AR2" s="1">
         <v>-290.53958755466402</v>
       </c>
-      <c r="AR2" s="3">
+      <c r="AS2" s="1">
         <v>-312.03951703370916</v>
       </c>
-      <c r="AS2" s="3">
+      <c r="AT2" s="1">
         <v>-333.57024370903508</v>
       </c>
-      <c r="AT2" s="3">
+      <c r="AU2" s="1">
         <v>-354.91873930641339</v>
       </c>
-      <c r="AU2" s="3">
+      <c r="AV2" s="1">
         <v>-375.5040261861854</v>
       </c>
-      <c r="AV2" s="3">
+      <c r="AW2" s="1">
         <v>-395.03023554786711</v>
       </c>
-      <c r="AW2" s="3">
+      <c r="AX2" s="1">
         <v>-412.41156591197324</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="AY2" s="1">
         <v>-426.84597071889226</v>
       </c>
-      <c r="AY2" s="3">
+      <c r="AZ2" s="1">
         <v>-437.09027401614566</v>
       </c>
-      <c r="AZ2" s="3">
+      <c r="BA2" s="1">
         <v>-442.33535730433942</v>
       </c>
-      <c r="BA2" s="3">
+      <c r="BB2" s="1">
         <v>-443.66236337625242</v>
       </c>
-      <c r="BB2" s="3">
+      <c r="BC2" s="1">
         <v>-441.0003891959949</v>
       </c>
-      <c r="BC2" s="3">
+      <c r="BD2" s="1">
         <v>-430.41637985529104</v>
       </c>
-      <c r="BD2" s="3">
+      <c r="BE2" s="1">
         <v>-402.00889878484179</v>
       </c>
-      <c r="BE2" s="3">
+      <c r="BF2" s="1">
         <v>-365.02408009663634</v>
       </c>
-      <c r="BF2" s="3">
+      <c r="BG2" s="1">
         <v>-320.49114232484669</v>
       </c>
-      <c r="BG2" s="3">
+      <c r="BH2" s="1">
         <v>-270.17403297984578</v>
       </c>
-      <c r="BH2" s="3">
+      <c r="BI2" s="1">
         <v>-216.94974848281615</v>
       </c>
-      <c r="BI2" s="3">
+      <c r="BJ2" s="1">
         <v>-163.36316060756056</v>
       </c>
-      <c r="BJ2" s="3">
+      <c r="BK2" s="1">
         <v>-113.21067030103946</v>
       </c>
-      <c r="BK2" s="3">
+      <c r="BL2" s="1">
         <v>-70.530247597547586</v>
       </c>
-      <c r="BL2" s="3">
+      <c r="BM2" s="1">
         <v>-36.675728750724744</v>
       </c>
-      <c r="BM2" s="3">
+      <c r="BN2" s="1">
         <v>-11.002718625217421</v>
       </c>
-      <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1"/>
@@ -1953,204 +1964,207 @@
       <c r="BS2" s="1"/>
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
-    </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
+      <c r="BV2" s="1"/>
+    </row>
+    <row r="3" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
       <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="1">
         <v>-57.954226889600008</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="1">
         <v>-58.115005030308943</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="1">
         <v>-58.273911282129106</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="1">
         <v>-58.481577887919237</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="1">
         <v>-58.743304465405892</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="1">
         <v>-59.061635976328894</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="1">
         <v>-59.438392964815989</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="1">
         <v>-59.875192955398816</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="1">
         <v>-60.373645035928448</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="1">
         <v>-60.935440599983366</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="1">
         <v>-61.562403484027946</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="1">
         <v>-62.334295744373954</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="1">
         <v>-63.237881102929123</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="1">
         <v>-64.278913330244492</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="1">
         <v>-65.463877647359524</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="1">
         <v>-66.800113775993609</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="1">
         <v>-68.295921490061218</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="1">
         <v>-69.960663299784329</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="1">
         <v>-71.969167669658788</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="1">
         <v>-74.319830488016123</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="1">
         <v>-77.041708850609538</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="1">
         <v>-80.168983910027094</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="1">
         <v>-83.741705729537699</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="1">
         <v>-87.806655331496756</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="1">
         <v>-92.418357550095308</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="1">
         <v>-97.640278728983603</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="1">
         <v>-103.65558160091042</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="1">
         <v>-110.55746655334546</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AH3" s="1">
         <v>-118.46955107053421</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AI3" s="1">
         <v>-127.53816239310609</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AJ3" s="1">
         <v>-137.93666479197122</v>
       </c>
-      <c r="AJ3" s="3">
+      <c r="AK3" s="1">
         <v>-149.87072630586198</v>
       </c>
-      <c r="AK3" s="3">
+      <c r="AL3" s="1">
         <v>-163.58474119791092</v>
       </c>
-      <c r="AL3" s="3">
+      <c r="AM3" s="1">
         <v>-179.36967788316346</v>
       </c>
-      <c r="AM3" s="3">
+      <c r="AN3" s="1">
         <v>-196.19535176290515</v>
       </c>
-      <c r="AN3" s="3">
+      <c r="AO3" s="1">
         <v>-213.99095552652165</v>
       </c>
-      <c r="AO3" s="3">
+      <c r="AP3" s="1">
         <v>-232.52221178795477</v>
       </c>
-      <c r="AP3" s="3">
+      <c r="AQ3" s="1">
         <v>-251.7262982942178</v>
       </c>
-      <c r="AQ3" s="3">
+      <c r="AR3" s="1">
         <v>-271.50738548509895</v>
       </c>
-      <c r="AR3" s="3">
+      <c r="AS3" s="1">
         <v>-291.4534733278652</v>
       </c>
-      <c r="AS3" s="3">
+      <c r="AT3" s="1">
         <v>-311.40291951052541</v>
       </c>
-      <c r="AT3" s="3">
+      <c r="AU3" s="1">
         <v>-331.15524751664282</v>
       </c>
-      <c r="AU3" s="3">
+      <c r="AV3" s="1">
         <v>-350.12698264763401</v>
       </c>
-      <c r="AV3" s="3">
+      <c r="AW3" s="1">
         <v>-368.07291355186152</v>
       </c>
-      <c r="AW3" s="3">
+      <c r="AX3" s="1">
         <v>-383.87951445222291</v>
       </c>
-      <c r="AX3" s="3">
+      <c r="AY3" s="1">
         <v>-396.8161188777122</v>
       </c>
-      <c r="AY3" s="3">
+      <c r="AZ3" s="1">
         <v>-405.61477303464562</v>
       </c>
-      <c r="AZ3" s="3">
+      <c r="BA3" s="1">
         <v>-409.44717650918449</v>
       </c>
-      <c r="BA3" s="3">
+      <c r="BB3" s="1">
         <v>-409.42244617243216</v>
       </c>
-      <c r="BB3" s="3">
+      <c r="BC3" s="1">
         <v>-407.48183662086899</v>
       </c>
-      <c r="BC3" s="3">
+      <c r="BD3" s="1">
         <v>-399.4214756170685</v>
       </c>
-      <c r="BD3" s="3">
+      <c r="BE3" s="1">
         <v>-375.17380961904433</v>
       </c>
-      <c r="BE3" s="3">
+      <c r="BF3" s="1">
         <v>-341.53139227768099</v>
       </c>
-      <c r="BF3" s="3">
+      <c r="BG3" s="1">
         <v>-300.62428140403415</v>
       </c>
-      <c r="BG3" s="3">
+      <c r="BH3" s="1">
         <v>-254.08032791839653</v>
       </c>
-      <c r="BH3" s="3">
+      <c r="BI3" s="1">
         <v>-204.55917761185191</v>
       </c>
-      <c r="BI3" s="3">
+      <c r="BJ3" s="1">
         <v>-154.48074533958734</v>
       </c>
-      <c r="BJ3" s="3">
+      <c r="BK3" s="1">
         <v>-107.38840722556688</v>
       </c>
-      <c r="BK3" s="3">
+      <c r="BL3" s="1">
         <v>-67.120931264027675</v>
       </c>
-      <c r="BL3" s="3">
+      <c r="BM3" s="1">
         <v>-35.051944484265356</v>
       </c>
-      <c r="BM3" s="3">
+      <c r="BN3" s="1">
         <v>-10.597193001740688</v>
       </c>
-      <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
@@ -2158,204 +2172,207 @@
       <c r="BS3" s="1"/>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
-    </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
+      <c r="BV3" s="1"/>
+    </row>
+    <row r="4" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="1">
         <v>-62.993724880000002</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="1">
         <v>-63.168483728596676</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="1">
         <v>-63.341207915357721</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="1">
         <v>-63.56693248686873</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="1">
         <v>-63.851417897180312</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="1">
         <v>-64.19743040905314</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="1">
         <v>-64.606948874799983</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="1">
         <v>-65.08173147325958</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="1">
         <v>-65.623527212965698</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="1">
         <v>-66.234174565199311</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="1">
         <v>-66.91565596089994</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="1">
         <v>-67.754669287362987</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="1">
         <v>-68.736827285792515</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="1">
         <v>-69.868384054613585</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="1">
         <v>-71.15638874712991</v>
       </c>
-      <c r="T4" s="3">
+      <c r="U4" s="1">
         <v>-72.608819321732184</v>
       </c>
-      <c r="U4" s="3">
+      <c r="V4" s="1">
         <v>-74.234697271805672</v>
       </c>
-      <c r="V4" s="3">
+      <c r="W4" s="1">
         <v>-76.044199238896013</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="1">
         <v>-78.227356162672592</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Y4" s="1">
         <v>-80.782424443495785</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Z4" s="1">
         <v>-83.740987881097325</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AA4" s="1">
         <v>-87.140199902203364</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="1">
         <v>-91.023593184280102</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AC4" s="1">
         <v>-95.442016664670376</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AD4" s="1">
         <v>-100.4547364674949</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AE4" s="1">
         <v>-106.13073774889521</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AF4" s="1">
         <v>-112.66911043577218</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AG4" s="1">
         <v>-120.17115929711463</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AH4" s="1">
         <v>-128.77125116362413</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AI4" s="1">
         <v>-138.62843738381096</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AJ4" s="1">
         <v>-149.9311573825774</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AK4" s="1">
         <v>-162.90296337593691</v>
       </c>
-      <c r="AK4" s="3">
+      <c r="AL4" s="1">
         <v>-177.80950130207708</v>
       </c>
-      <c r="AL4" s="3">
+      <c r="AM4" s="1">
         <v>-194.96704117735158</v>
       </c>
-      <c r="AM4" s="3">
+      <c r="AN4" s="1">
         <v>-213.25581713359253</v>
       </c>
-      <c r="AN4" s="3">
+      <c r="AO4" s="1">
         <v>-232.59886470274088</v>
       </c>
-      <c r="AO4" s="3">
+      <c r="AP4" s="1">
         <v>-252.74153455212476</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AQ4" s="1">
         <v>-273.61554162414973</v>
       </c>
-      <c r="AQ4" s="3">
+      <c r="AR4" s="1">
         <v>-295.1167233533684</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AS4" s="1">
         <v>-316.79725361724473</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AT4" s="1">
         <v>-338.48143425057111</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AU4" s="1">
         <v>-359.95135599635086</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AV4" s="1">
         <v>-380.57280722568913</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AW4" s="1">
         <v>-400.07925386071901</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AX4" s="1">
         <v>-417.26034179589442</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AY4" s="1">
         <v>-431.32186834533934</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AZ4" s="1">
         <v>-440.88562286374525</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="BA4" s="1">
         <v>-445.05127881433089</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BB4" s="1">
         <v>-445.02439801351318</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BC4" s="1">
         <v>-442.91503980529239</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BD4" s="1">
         <v>-434.15377784463965</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BE4" s="1">
         <v>-407.79761915113517</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BF4" s="1">
         <v>-371.22977421487059</v>
       </c>
-      <c r="BF4" s="3">
+      <c r="BG4" s="1">
         <v>-326.76552326525456</v>
       </c>
-      <c r="BG4" s="3">
+      <c r="BH4" s="1">
         <v>-276.17426947651796</v>
       </c>
-      <c r="BH4" s="3">
+      <c r="BI4" s="1">
         <v>-222.34693218679553</v>
       </c>
-      <c r="BI4" s="3">
+      <c r="BJ4" s="1">
         <v>-167.91385362998625</v>
       </c>
-      <c r="BJ4" s="3">
+      <c r="BK4" s="1">
         <v>-116.72652959300748</v>
       </c>
-      <c r="BK4" s="3">
+      <c r="BL4" s="1">
         <v>-72.957533982638779</v>
       </c>
-      <c r="BL4" s="3">
+      <c r="BM4" s="1">
         <v>-38.099939656810172</v>
       </c>
-      <c r="BM4" s="3">
+      <c r="BN4" s="1">
         <v>-11.518688045370313</v>
       </c>
-      <c r="BN4" s="1"/>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
@@ -2363,204 +2380,207 @@
       <c r="BS4" s="1"/>
       <c r="BT4" s="1"/>
       <c r="BU4" s="1"/>
-    </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
+      <c r="BV4" s="1"/>
+    </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="1">
         <v>-62.993724880000002</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="1">
         <v>-63.168483728596676</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="1">
         <v>-63.341207915357721</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="1">
         <v>-63.56693248686873</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="1">
         <v>-63.851417897180312</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="1">
         <v>-64.19743040905314</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="1">
         <v>-64.606948874799983</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="1">
         <v>-65.08173147325958</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="1">
         <v>-65.623527212965698</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="1">
         <v>-66.234174565199311</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="1">
         <v>-66.91565596089994</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="1">
         <v>-67.754669287362987</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="1">
         <v>-68.736827285792515</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="1">
         <v>-69.868384054613585</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="1">
         <v>-71.15638874712991</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="1">
         <v>-72.608819321732184</v>
       </c>
-      <c r="U5" s="3">
+      <c r="V5" s="1">
         <v>-74.234697271805672</v>
       </c>
-      <c r="V5" s="3">
+      <c r="W5" s="1">
         <v>-76.044199238896013</v>
       </c>
-      <c r="W5" s="3">
+      <c r="X5" s="1">
         <v>-78.227356162672592</v>
       </c>
-      <c r="X5" s="3">
+      <c r="Y5" s="1">
         <v>-80.782424443495785</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Z5" s="1">
         <v>-83.740987881097325</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="AA5" s="1">
         <v>-87.140199902203364</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AB5" s="1">
         <v>-91.023593184280102</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AC5" s="1">
         <v>-95.442016664670376</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="AD5" s="1">
         <v>-100.4547364674949</v>
       </c>
-      <c r="AD5" s="3">
+      <c r="AE5" s="1">
         <v>-106.13073774889521</v>
       </c>
-      <c r="AE5" s="3">
+      <c r="AF5" s="1">
         <v>-112.66911043577218</v>
       </c>
-      <c r="AF5" s="3">
+      <c r="AG5" s="1">
         <v>-120.17115929711463</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AH5" s="1">
         <v>-128.77125116362413</v>
       </c>
-      <c r="AH5" s="3">
+      <c r="AI5" s="1">
         <v>-138.62843738381096</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AJ5" s="1">
         <v>-149.9311573825774</v>
       </c>
-      <c r="AJ5" s="3">
+      <c r="AK5" s="1">
         <v>-162.90296337593691</v>
       </c>
-      <c r="AK5" s="3">
+      <c r="AL5" s="1">
         <v>-177.80950130207708</v>
       </c>
-      <c r="AL5" s="3">
+      <c r="AM5" s="1">
         <v>-194.96704117735158</v>
       </c>
-      <c r="AM5" s="3">
+      <c r="AN5" s="1">
         <v>-213.25581713359253</v>
       </c>
-      <c r="AN5" s="3">
+      <c r="AO5" s="1">
         <v>-232.59886470274088</v>
       </c>
-      <c r="AO5" s="3">
+      <c r="AP5" s="1">
         <v>-252.74153455212476</v>
       </c>
-      <c r="AP5" s="3">
+      <c r="AQ5" s="1">
         <v>-273.61554162414973</v>
       </c>
-      <c r="AQ5" s="3">
+      <c r="AR5" s="1">
         <v>-295.1167233533684</v>
       </c>
-      <c r="AR5" s="3">
+      <c r="AS5" s="1">
         <v>-316.79725361724473</v>
       </c>
-      <c r="AS5" s="3">
+      <c r="AT5" s="1">
         <v>-338.48143425057111</v>
       </c>
-      <c r="AT5" s="3">
+      <c r="AU5" s="1">
         <v>-359.95135599635086</v>
       </c>
-      <c r="AU5" s="3">
+      <c r="AV5" s="1">
         <v>-380.57280722568913</v>
       </c>
-      <c r="AV5" s="3">
+      <c r="AW5" s="1">
         <v>-400.07925386071901</v>
       </c>
-      <c r="AW5" s="3">
+      <c r="AX5" s="1">
         <v>-417.26034179589442</v>
       </c>
-      <c r="AX5" s="3">
+      <c r="AY5" s="1">
         <v>-431.32186834533934</v>
       </c>
-      <c r="AY5" s="3">
+      <c r="AZ5" s="1">
         <v>-440.88562286374525</v>
       </c>
-      <c r="AZ5" s="3">
+      <c r="BA5" s="1">
         <v>-445.05127881433089</v>
       </c>
-      <c r="BA5" s="3">
+      <c r="BB5" s="1">
         <v>-445.02439801351318</v>
       </c>
-      <c r="BB5" s="3">
+      <c r="BC5" s="1">
         <v>-442.91503980529239</v>
       </c>
-      <c r="BC5" s="3">
+      <c r="BD5" s="1">
         <v>-434.15377784463965</v>
       </c>
-      <c r="BD5" s="3">
+      <c r="BE5" s="1">
         <v>-407.79761915113517</v>
       </c>
-      <c r="BE5" s="3">
+      <c r="BF5" s="1">
         <v>-371.22977421487059</v>
       </c>
-      <c r="BF5" s="3">
+      <c r="BG5" s="1">
         <v>-326.76552326525456</v>
       </c>
-      <c r="BG5" s="3">
+      <c r="BH5" s="1">
         <v>-276.17426947651796</v>
       </c>
-      <c r="BH5" s="3">
+      <c r="BI5" s="1">
         <v>-222.34693218679553</v>
       </c>
-      <c r="BI5" s="3">
+      <c r="BJ5" s="1">
         <v>-167.91385362998625</v>
       </c>
-      <c r="BJ5" s="3">
+      <c r="BK5" s="1">
         <v>-116.72652959300748</v>
       </c>
-      <c r="BK5" s="3">
+      <c r="BL5" s="1">
         <v>-72.957533982638779</v>
       </c>
-      <c r="BL5" s="3">
+      <c r="BM5" s="1">
         <v>-38.099939656810172</v>
       </c>
-      <c r="BM5" s="3">
+      <c r="BN5" s="1">
         <v>-11.518688045370313</v>
       </c>
-      <c r="BN5" s="1"/>
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
@@ -2568,204 +2588,207 @@
       <c r="BS5" s="1"/>
       <c r="BT5" s="1"/>
       <c r="BU5" s="1"/>
-    </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
+      <c r="BV5" s="1"/>
+    </row>
+    <row r="6" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>1566.5712585016952</v>
       </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>1409.9141326515257</v>
       </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
         <v>1268.922719386373</v>
       </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
         <v>1142.0304474477359</v>
       </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3">
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
         <v>1027.8274027029622</v>
       </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
         <v>925.04466243266609</v>
       </c>
-      <c r="X6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="3">
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
         <v>832.54019618939947</v>
       </c>
-      <c r="AA6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="3">
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
         <v>749.28617657045959</v>
       </c>
-      <c r="AD6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="3">
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
         <v>674.35755891341364</v>
       </c>
-      <c r="AG6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="3">
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
         <v>606.92180302207225</v>
       </c>
-      <c r="AJ6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="3">
+      <c r="AK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
         <v>546.22962271986512</v>
       </c>
-      <c r="AM6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="3">
+      <c r="AN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="1">
         <v>491.60666044787865</v>
       </c>
-      <c r="AP6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="3">
+      <c r="AQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="1">
         <v>437.52992779861199</v>
       </c>
-      <c r="AS6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="3">
+      <c r="AT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="1">
         <v>380.65103718479241</v>
       </c>
-      <c r="AV6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="3">
+      <c r="AW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="1">
         <v>319.74687123522563</v>
       </c>
-      <c r="AY6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="3">
+      <c r="AZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="1">
         <v>255.79749698818051</v>
       </c>
-      <c r="BB6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="3">
+      <c r="BC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="1">
         <v>191.84812274113537</v>
       </c>
-      <c r="BE6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG6" s="3">
+      <c r="BF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="1">
         <v>132.3752046913834</v>
       </c>
-      <c r="BH6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="3">
+      <c r="BI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="1">
         <v>82.07262690865771</v>
       </c>
-      <c r="BK6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM6" s="3">
+      <c r="BL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="1">
         <v>44.319218530675165</v>
       </c>
-      <c r="BN6" s="1"/>
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
@@ -2773,204 +2796,207 @@
       <c r="BS6" s="1"/>
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
-    </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A7" s="2" t="s">
+      <c r="BV6" s="1"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
         <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
         <v>1624.6251068288839</v>
       </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>1482.5636172728382</v>
       </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3">
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
         <v>1345.9329414827955</v>
       </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
         <v>1219.0134272989244</v>
       </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
         <v>1102.5686739919304</v>
       </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3">
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
         <v>996.37180841886288</v>
       </c>
-      <c r="X7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="3">
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
         <v>899.76145445990721</v>
       </c>
-      <c r="AA7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="3">
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
         <v>811.95685330102481</v>
       </c>
-      <c r="AD7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3">
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
         <v>732.39989508648955</v>
       </c>
-      <c r="AG7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="3">
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
         <v>660.41015192801819</v>
       </c>
-      <c r="AJ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="3">
+      <c r="AK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
         <v>595.20791972018378</v>
       </c>
-      <c r="AM7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="3">
+      <c r="AN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="1">
         <v>536.25982958350767</v>
       </c>
-      <c r="AP7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="3">
+      <c r="AQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="1">
         <v>477.54800913342808</v>
       </c>
-      <c r="AS7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="3">
+      <c r="AT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="1">
         <v>415.33374099674052</v>
       </c>
-      <c r="AV7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="3">
+      <c r="AW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="1">
         <v>347.64307801101478</v>
       </c>
-      <c r="AY7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="3">
+      <c r="AZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="1">
         <v>270.07692844608704</v>
       </c>
-      <c r="BB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD7" s="3">
+      <c r="BC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
         <v>212.3423705797934</v>
       </c>
-      <c r="BE7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG7" s="3">
+      <c r="BF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="1">
         <v>149.40149408439092</v>
       </c>
-      <c r="BH7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="3">
+      <c r="BI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="1">
         <v>94.020777736826616</v>
       </c>
-      <c r="BK7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM7" s="3">
+      <c r="BL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="1">
         <v>51.697238455499402</v>
       </c>
-      <c r="BN7" s="1"/>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
@@ -2978,204 +3004,207 @@
       <c r="BS7" s="1"/>
       <c r="BT7" s="1"/>
       <c r="BU7" s="1"/>
-    </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A8" s="2" t="s">
+      <c r="BV7" s="1"/>
+    </row>
+    <row r="8" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
         <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
         <v>1524.4889327417729</v>
       </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
         <v>1355.503226622239</v>
       </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3">
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
         <v>1210.0723192327061</v>
       </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
         <v>1082.3404993092172</v>
       </c>
-      <c r="R8" s="3">
-        <v>0</v>
-      </c>
-      <c r="S8" s="3">
-        <v>0</v>
-      </c>
-      <c r="T8" s="3">
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
         <v>969.21563668104034</v>
       </c>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3">
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
         <v>868.58955265352063</v>
       </c>
-      <c r="X8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3">
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
         <v>778.92839139009402</v>
       </c>
-      <c r="AA8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="3">
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
         <v>699.00155941208368</v>
       </c>
-      <c r="AD8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3">
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
         <v>627.5519551203879</v>
       </c>
-      <c r="AG8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="3">
+      <c r="AH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1">
         <v>563.60529048172896</v>
       </c>
-      <c r="AJ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="3">
+      <c r="AK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="1">
         <v>506.44039555644883</v>
       </c>
-      <c r="AM8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="3">
+      <c r="AN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="1">
         <v>455.24458098732691</v>
       </c>
-      <c r="AP8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="3">
+      <c r="AQ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="1">
         <v>404.90020182369005</v>
       </c>
-      <c r="AS8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="3">
+      <c r="AT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1">
         <v>352.39180200760774</v>
       </c>
-      <c r="AV8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="3">
+      <c r="AW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="1">
         <v>297.19676728190313</v>
       </c>
-      <c r="AY8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="3">
+      <c r="AZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="1">
         <v>245.00088084392468</v>
       </c>
-      <c r="BB8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="3">
+      <c r="BC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="1">
         <v>174.6139985752873</v>
       </c>
-      <c r="BE8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="3">
+      <c r="BF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="1">
         <v>117.44013187254799</v>
       </c>
-      <c r="BH8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="3">
+      <c r="BI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="1">
         <v>71.25496413580359</v>
       </c>
-      <c r="BK8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM8" s="3">
+      <c r="BL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="1">
         <v>37.382874720276277</v>
       </c>
-      <c r="BN8" s="1"/>
       <c r="BO8" s="1"/>
       <c r="BP8" s="1"/>
       <c r="BQ8" s="1"/>
@@ -3183,204 +3212,207 @@
       <c r="BS8" s="1"/>
       <c r="BT8" s="1"/>
       <c r="BU8" s="1"/>
-    </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.5">
-      <c r="A9" s="2" t="s">
+      <c r="BV8" s="1"/>
+    </row>
+    <row r="9" spans="1:74" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
         <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="1">
         <v>1740.6347316685503</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
         <v>1524.4889327417729</v>
       </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>1355.503226622239</v>
       </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
         <v>1210.0723192327061</v>
       </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3">
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
         <v>1082.3404993092172</v>
       </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
-      <c r="T9" s="3">
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
         <v>969.21563668104034</v>
       </c>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
-      <c r="V9" s="3">
-        <v>0</v>
-      </c>
-      <c r="W9" s="3">
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
         <v>868.58955265352063</v>
       </c>
-      <c r="X9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="3">
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
         <v>778.92839139009402</v>
       </c>
-      <c r="AA9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="3">
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
         <v>699.00155941208368</v>
       </c>
-      <c r="AD9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3">
+      <c r="AE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1">
         <v>627.5519551203879</v>
       </c>
-      <c r="AG9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="3">
+      <c r="AH9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1">
         <v>563.60529048172896</v>
       </c>
-      <c r="AJ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="3">
+      <c r="AK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1">
         <v>506.44039555644883</v>
       </c>
-      <c r="AM9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="3">
+      <c r="AN9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1">
         <v>455.24458098732691</v>
       </c>
-      <c r="AP9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="3">
+      <c r="AQ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="1">
         <v>404.90020182369005</v>
       </c>
-      <c r="AS9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="3">
+      <c r="AT9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="1">
         <v>352.39180200760774</v>
       </c>
-      <c r="AV9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="3">
+      <c r="AW9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="1">
         <v>297.19676728190313</v>
       </c>
-      <c r="AY9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="3">
+      <c r="AZ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="1">
         <v>245.00088084392468</v>
       </c>
-      <c r="BB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD9" s="3">
+      <c r="BC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="1">
         <v>174.6139985752873</v>
       </c>
-      <c r="BE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BF9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="3">
+      <c r="BF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="1">
         <v>117.44013187254799</v>
       </c>
-      <c r="BH9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BI9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="3">
+      <c r="BI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="1">
         <v>71.25496413580359</v>
       </c>
-      <c r="BK9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM9" s="3">
+      <c r="BL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="1">
         <v>37.382874720276277</v>
       </c>
-      <c r="BN9" s="1"/>
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
       <c r="BQ9" s="1"/>
@@ -3388,6 +3420,7 @@
       <c r="BS9" s="1"/>
       <c r="BT9" s="1"/>
       <c r="BU9" s="1"/>
+      <c r="BV9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3395,20 +3428,20 @@
     <dataValidation type="list" allowBlank="1" sqref="A2:A9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>GroupOfContract_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B9" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:C9" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>AmountType_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C9" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>VariableType_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E9" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>Novelty_SystemName</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B6:C6 D3 C2 D2" numberStoredAsText="1" calculatedColumn="1"/>
+    <ignoredError sqref="D6 E3 D2:E2 B6" numberStoredAsText="1" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>